<commit_message>
Actualizacion Viaticos_q_plan de proyecto
</commit_message>
<xml_diff>
--- a/Proyectos/Activos/Viaticos_q/2. Estimacion y planeacion/2. Planeacion/Viaticos_q_Plan_Proyecto.xlsx
+++ b/Proyectos/Activos/Viaticos_q/2. Estimacion y planeacion/2. Planeacion/Viaticos_q_Plan_Proyecto.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\IWM\Repositorio IWM\Proyectos\Activos\Viaticos_q\2. Estimacion y planeacion\2. Plantillas planeacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\IWM\Repositorio IWM\Proyectos\Activos\Viaticos_q\2. Estimacion y planeacion\2. Planeacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="875" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="875"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Generales" sheetId="23" r:id="rId1"/>
@@ -552,9 +552,6 @@
     <t>Nombre del Proyecto:</t>
   </si>
   <si>
-    <t>&lt;Nombre del Proyecto&gt;</t>
-  </si>
-  <si>
     <t>Empresa:</t>
   </si>
   <si>
@@ -1463,6 +1460,9 @@
   </si>
   <si>
     <t>Ejecución del plan de pruebas</t>
+  </si>
+  <si>
+    <t>Viaticos</t>
   </si>
 </sst>
 </file>
@@ -2926,21 +2926,24 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="12" xfId="52" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="37" fillId="24" borderId="0" xfId="54" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="24" borderId="0" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="11" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="27" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="31" fillId="25" borderId="0" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="25" borderId="10" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="27" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="24" borderId="0" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -2967,9 +2970,6 @@
     </xf>
     <xf numFmtId="0" fontId="31" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="24" borderId="0" xfId="54" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="56">
@@ -3807,8 +3807,8 @@
   </sheetPr>
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28:C28"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -4075,7 +4075,7 @@
     <row r="2" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="145"/>
       <c r="B2" s="144" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="145"/>
       <c r="D2" s="77"/>
@@ -4087,7 +4087,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="177" t="s">
-        <v>4</v>
+        <v>306</v>
       </c>
       <c r="D3" s="178"/>
       <c r="E3" s="178"/>
@@ -4095,10 +4095,10 @@
     <row r="4" spans="1:7" s="70" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" s="79" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D4" s="80"/>
       <c r="E4" s="80"/>
@@ -4106,7 +4106,7 @@
     <row r="5" spans="1:7" s="70" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="146"/>
       <c r="B5" s="145" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="146"/>
       <c r="D5" s="78"/>
@@ -4115,10 +4115,10 @@
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="74" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D6" s="76"/>
       <c r="E6" s="76"/>
@@ -4126,7 +4126,7 @@
     <row r="7" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" s="161">
         <v>42199</v>
@@ -4139,38 +4139,38 @@
     <row r="8" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="147"/>
       <c r="B8" s="144" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" s="147"/>
     </row>
     <row r="9" spans="1:7" ht="12.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B9" s="65" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" s="98" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E9" s="115" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F9" s="115" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="12.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B10" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="69" t="s">
         <v>23</v>
-      </c>
-      <c r="C10" s="69" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="42.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B11" s="65" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" s="64" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -4180,90 +4180,90 @@
     <row r="13" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="147"/>
       <c r="B13" s="144" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" s="147"/>
     </row>
     <row r="14" spans="1:7" ht="12.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B14" s="61" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="66" t="s">
         <v>27</v>
-      </c>
-      <c r="C14" s="66" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B15" s="181" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C15" s="64" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="16" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B16" s="182"/>
       <c r="C16" s="67" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="17" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B17" s="183" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C17" s="62" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="18" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B18" s="182"/>
       <c r="C18" s="62" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="19" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B19" s="183" t="s">
+        <v>244</v>
+      </c>
+      <c r="C19" s="62" t="s">
         <v>245</v>
-      </c>
-      <c r="C19" s="62" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="20" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B20" s="181"/>
       <c r="C20" s="62" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="21" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B21" s="181"/>
       <c r="C21" s="62" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="22" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B22" s="181"/>
       <c r="C22" s="62" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="23" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B23" s="182"/>
       <c r="C23" s="62" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="24" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B24" s="183" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C24" s="62" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="25" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B25" s="182"/>
       <c r="C25" s="62" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -4273,26 +4273,26 @@
     <row r="27" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A27" s="147"/>
       <c r="B27" s="144" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C27" s="147"/>
     </row>
     <row r="28" spans="1:3" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="179" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C28" s="180"/>
     </row>
     <row r="29" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A29" s="147"/>
       <c r="B29" s="144" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C29" s="147"/>
     </row>
     <row r="30" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="179" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C30" s="179"/>
     </row>
@@ -4330,8 +4330,8 @@
   </sheetPr>
   <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A37" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView showGridLines="0" topLeftCell="A7" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -4790,7 +4790,7 @@
     <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="148"/>
       <c r="B2" s="149" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C2" s="148"/>
       <c r="D2" s="148"/>
@@ -4801,7 +4801,7 @@
     <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="155"/>
       <c r="B3" s="156" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C3" s="155"/>
       <c r="D3" s="155"/>
@@ -4818,37 +4818,37 @@
         <v>0</v>
       </c>
       <c r="D4" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="25" t="s">
-        <v>17</v>
-      </c>
       <c r="F4" s="25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G4" s="25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="38.25" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A5" s="15"/>
       <c r="B5" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="E5" s="162" t="s">
+        <v>166</v>
+      </c>
+      <c r="F5" s="18" t="s">
         <v>165</v>
       </c>
-      <c r="C5" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>168</v>
-      </c>
-      <c r="E5" s="162" t="s">
-        <v>167</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>166</v>
-      </c>
       <c r="G5" s="19" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="6" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -4863,7 +4863,7 @@
     <row r="7" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A7" s="146"/>
       <c r="B7" s="150" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" s="146"/>
       <c r="D7" s="146"/>
@@ -4876,20 +4876,20 @@
       <c r="B8" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="185" t="s">
+      <c r="C8" s="188" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="188"/>
+      <c r="E8" s="189" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="185"/>
-      <c r="E8" s="186" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="186"/>
+      <c r="F8" s="189"/>
       <c r="G8" s="25"/>
     </row>
     <row r="9" spans="1:7" ht="18.75" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A9" s="151"/>
       <c r="B9" s="152" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C9" s="152"/>
       <c r="D9" s="152"/>
@@ -4900,26 +4900,26 @@
     <row r="10" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A10" s="26"/>
       <c r="B10" s="21" t="s">
-        <v>179</v>
-      </c>
-      <c r="C10" s="184" t="str">
+        <v>178</v>
+      </c>
+      <c r="C10" s="186" t="str">
         <f>VLOOKUP(B10,$B$50:$D$66,2,0)</f>
         <v>33 1605 3573</v>
       </c>
-      <c r="D10" s="184"/>
-      <c r="E10" s="184" t="str">
+      <c r="D10" s="186"/>
+      <c r="E10" s="186" t="str">
         <f>VLOOKUP(B10,$B$50:$D$66,3,0)</f>
         <v>felipelozanopadilla@gmail.com</v>
       </c>
-      <c r="F10" s="184"/>
+      <c r="F10" s="186"/>
       <c r="G10" s="163" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="24.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A11" s="153"/>
       <c r="B11" s="154" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C11" s="154"/>
       <c r="D11" s="154"/>
@@ -4930,26 +4930,26 @@
     <row r="12" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26"/>
       <c r="B12" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="C12" s="184" t="str">
+        <v>168</v>
+      </c>
+      <c r="C12" s="186" t="str">
         <f>VLOOKUP(B12,$B$50:$D$66,2,0)</f>
         <v>33 3504 5902</v>
       </c>
-      <c r="D12" s="184"/>
-      <c r="E12" s="184" t="str">
+      <c r="D12" s="186"/>
+      <c r="E12" s="186" t="str">
         <f>VLOOKUP(B12,$B$50:$D$66,3,0)</f>
         <v>charles.gonher@gmail.com</v>
       </c>
-      <c r="F12" s="184"/>
+      <c r="F12" s="186"/>
       <c r="G12" s="163" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="24.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13" s="153"/>
       <c r="B13" s="154" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C13" s="154"/>
       <c r="D13" s="154"/>
@@ -4960,43 +4960,43 @@
     <row r="14" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A14" s="26"/>
       <c r="B14" s="21" t="s">
-        <v>164</v>
-      </c>
-      <c r="C14" s="184" t="str">
+        <v>163</v>
+      </c>
+      <c r="C14" s="186" t="str">
         <f>VLOOKUP(B14,$B$50:$D$66,2,0)</f>
         <v>33 1862 1719</v>
       </c>
-      <c r="D14" s="184"/>
-      <c r="E14" s="184" t="str">
+      <c r="D14" s="186"/>
+      <c r="E14" s="186" t="str">
         <f>VLOOKUP(B14,$B$50:$D$66,3,0)</f>
         <v>rpulido@qualtop.com</v>
       </c>
-      <c r="F14" s="184"/>
+      <c r="F14" s="186"/>
       <c r="G14" s="163" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A15" s="26"/>
       <c r="B15" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="C15" s="184" t="e">
+        <v>74</v>
+      </c>
+      <c r="C15" s="186" t="e">
         <f>VLOOKUP(B15,$B$50:$D$66,2,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="D15" s="184"/>
-      <c r="E15" s="184" t="e">
+      <c r="D15" s="186"/>
+      <c r="E15" s="186" t="e">
         <f>VLOOKUP(B15,$B$50:$D$66,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="F15" s="184"/>
+      <c r="F15" s="186"/>
       <c r="G15" s="23"/>
     </row>
     <row r="16" spans="1:7" ht="24.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16" s="153"/>
       <c r="B16" s="154" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C16" s="154"/>
       <c r="D16" s="154"/>
@@ -5007,60 +5007,60 @@
     <row r="17" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" s="26"/>
       <c r="B17" s="21" t="s">
-        <v>171</v>
-      </c>
-      <c r="C17" s="184" t="str">
+        <v>170</v>
+      </c>
+      <c r="C17" s="186" t="str">
         <f>VLOOKUP(B17,$B$50:$D$66,2,0)</f>
         <v>22 2752 8219</v>
       </c>
-      <c r="D17" s="184"/>
-      <c r="E17" s="184" t="str">
+      <c r="D17" s="186"/>
+      <c r="E17" s="186" t="str">
         <f>VLOOKUP(B17,$B$50:$D$66,3,0)</f>
         <v>jzepeda@qualtop.com</v>
       </c>
-      <c r="F17" s="184"/>
+      <c r="F17" s="186"/>
       <c r="G17" s="163" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A18" s="26"/>
       <c r="B18" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="C18" s="184" t="e">
+        <v>74</v>
+      </c>
+      <c r="C18" s="186" t="e">
         <f>VLOOKUP(B18,$B$50:$D$66,2,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="D18" s="184"/>
-      <c r="E18" s="184" t="e">
+      <c r="D18" s="186"/>
+      <c r="E18" s="186" t="e">
         <f>VLOOKUP(B18,$B$50:$D$66,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="F18" s="184"/>
+      <c r="F18" s="186"/>
       <c r="G18" s="23"/>
     </row>
     <row r="19" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A19" s="26"/>
       <c r="B19" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="C19" s="184" t="e">
+        <v>74</v>
+      </c>
+      <c r="C19" s="186" t="e">
         <f>VLOOKUP(B19,$B$50:$D$66,2,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="D19" s="184"/>
-      <c r="E19" s="184" t="e">
+      <c r="D19" s="186"/>
+      <c r="E19" s="186" t="e">
         <f>VLOOKUP(B19,$B$50:$D$66,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="F19" s="184"/>
+      <c r="F19" s="186"/>
       <c r="G19" s="23"/>
     </row>
     <row r="20" spans="1:7" ht="24.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A20" s="153"/>
       <c r="B20" s="154" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C20" s="154"/>
       <c r="D20" s="154"/>
@@ -5071,37 +5071,37 @@
     <row r="21" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A21" s="26"/>
       <c r="B21" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="C21" s="184" t="str">
+        <v>168</v>
+      </c>
+      <c r="C21" s="186" t="str">
         <f>VLOOKUP(B21,$B$50:$D$66,2,0)</f>
         <v>33 3504 5902</v>
       </c>
-      <c r="D21" s="184"/>
-      <c r="E21" s="184" t="str">
+      <c r="D21" s="186"/>
+      <c r="E21" s="186" t="str">
         <f>VLOOKUP(B21,$B$50:$D$66,3,0)</f>
         <v>charles.gonher@gmail.com</v>
       </c>
-      <c r="F21" s="184"/>
+      <c r="F21" s="186"/>
       <c r="G21" s="163" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A22" s="26"/>
       <c r="B22" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="C22" s="184" t="e">
+        <v>74</v>
+      </c>
+      <c r="C22" s="186" t="e">
         <f>VLOOKUP(B22,$B$50:$D$66,2,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="D22" s="184"/>
-      <c r="E22" s="184" t="e">
+      <c r="D22" s="186"/>
+      <c r="E22" s="186" t="e">
         <f>VLOOKUP(B22,$B$50:$D$66,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="F22" s="184"/>
+      <c r="F22" s="186"/>
       <c r="G22" s="23"/>
     </row>
     <row r="23" spans="1:7" ht="24.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -5118,26 +5118,26 @@
     <row r="24" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A24" s="26"/>
       <c r="B24" s="21" t="s">
-        <v>171</v>
-      </c>
-      <c r="C24" s="184" t="str">
+        <v>170</v>
+      </c>
+      <c r="C24" s="186" t="str">
         <f>VLOOKUP(B24,$B$50:$D$66,2,0)</f>
         <v>22 2752 8219</v>
       </c>
-      <c r="D24" s="184"/>
-      <c r="E24" s="184" t="str">
+      <c r="D24" s="186"/>
+      <c r="E24" s="186" t="str">
         <f>VLOOKUP(B24,$B$50:$D$66,3,0)</f>
         <v>jzepeda@qualtop.com</v>
       </c>
-      <c r="F24" s="184"/>
+      <c r="F24" s="186"/>
       <c r="G24" s="163" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="24.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A25" s="153"/>
       <c r="B25" s="154" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C25" s="154"/>
       <c r="D25" s="154"/>
@@ -5148,26 +5148,26 @@
     <row r="26" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A26" s="26"/>
       <c r="B26" s="21" t="s">
-        <v>171</v>
-      </c>
-      <c r="C26" s="184" t="str">
+        <v>170</v>
+      </c>
+      <c r="C26" s="186" t="str">
         <f>VLOOKUP(B26,$B$50:$D$66,2,0)</f>
         <v>22 2752 8219</v>
       </c>
-      <c r="D26" s="184"/>
-      <c r="E26" s="184" t="str">
+      <c r="D26" s="186"/>
+      <c r="E26" s="186" t="str">
         <f>VLOOKUP(B26,$B$50:$D$66,3,0)</f>
         <v>jzepeda@qualtop.com</v>
       </c>
-      <c r="F26" s="184"/>
+      <c r="F26" s="186"/>
       <c r="G26" s="163" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="24.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A27" s="153"/>
       <c r="B27" s="154" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C27" s="154"/>
       <c r="D27" s="154"/>
@@ -5178,26 +5178,26 @@
     <row r="28" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A28" s="26"/>
       <c r="B28" s="21" t="s">
-        <v>172</v>
-      </c>
-      <c r="C28" s="184" t="str">
+        <v>171</v>
+      </c>
+      <c r="C28" s="186" t="str">
         <f>VLOOKUP(B28,$B$50:$D$66,2,0)</f>
         <v>33 3807 6830</v>
       </c>
-      <c r="D28" s="184"/>
-      <c r="E28" s="184" t="str">
+      <c r="D28" s="186"/>
+      <c r="E28" s="186" t="str">
         <f>VLOOKUP(B28,$B$50:$D$66,3,0)</f>
         <v>asosa@qualtop.com</v>
       </c>
-      <c r="F28" s="184"/>
+      <c r="F28" s="186"/>
       <c r="G28" s="163" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="24.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A29" s="153"/>
       <c r="B29" s="154" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C29" s="154"/>
       <c r="D29" s="154"/>
@@ -5208,26 +5208,26 @@
     <row r="30" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A30" s="26"/>
       <c r="B30" s="21" t="s">
-        <v>172</v>
-      </c>
-      <c r="C30" s="184" t="str">
+        <v>171</v>
+      </c>
+      <c r="C30" s="186" t="str">
         <f>VLOOKUP(B30,$B$50:$D$66,2,0)</f>
         <v>33 3807 6830</v>
       </c>
-      <c r="D30" s="184"/>
-      <c r="E30" s="184" t="str">
+      <c r="D30" s="186"/>
+      <c r="E30" s="186" t="str">
         <f>VLOOKUP(B30,$B$50:$D$66,3,0)</f>
         <v>asosa@qualtop.com</v>
       </c>
-      <c r="F30" s="184"/>
+      <c r="F30" s="186"/>
       <c r="G30" s="163" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="24.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A31" s="153"/>
       <c r="B31" s="154" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C31" s="154"/>
       <c r="D31" s="154"/>
@@ -5238,26 +5238,26 @@
     <row r="32" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A32" s="26"/>
       <c r="B32" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="C32" s="184" t="str">
+        <v>168</v>
+      </c>
+      <c r="C32" s="186" t="str">
         <f>VLOOKUP(B32,$B$50:$D$66,2,0)</f>
         <v>33 3504 5902</v>
       </c>
-      <c r="D32" s="184"/>
-      <c r="E32" s="184" t="str">
+      <c r="D32" s="186"/>
+      <c r="E32" s="186" t="str">
         <f>VLOOKUP(B32,$B$50:$D$66,3,0)</f>
         <v>charles.gonher@gmail.com</v>
       </c>
-      <c r="F32" s="184"/>
+      <c r="F32" s="186"/>
       <c r="G32" s="163" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="24.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A33" s="153"/>
       <c r="B33" s="154" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C33" s="154"/>
       <c r="D33" s="154"/>
@@ -5268,7 +5268,7 @@
     <row r="34" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A34" s="26"/>
       <c r="B34" s="21" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C34" s="187" t="str">
         <f>VLOOKUP(B34,$B$50:$D$66,2,0)</f>
@@ -5281,13 +5281,13 @@
       </c>
       <c r="F34" s="187"/>
       <c r="G34" s="163" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="24.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A35" s="153"/>
       <c r="B35" s="154" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C35" s="154"/>
       <c r="D35" s="154"/>
@@ -5298,7 +5298,7 @@
     <row r="36" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A36" s="26"/>
       <c r="B36" s="21" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C36" s="187" t="str">
         <f>VLOOKUP(B36,$B$50:$D$66,2,0)</f>
@@ -5311,13 +5311,13 @@
       </c>
       <c r="F36" s="187"/>
       <c r="G36" s="163" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="24.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A37" s="153"/>
       <c r="B37" s="154" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C37" s="154"/>
       <c r="D37" s="154"/>
@@ -5328,26 +5328,26 @@
     <row r="38" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A38" s="26"/>
       <c r="B38" s="21" t="s">
-        <v>171</v>
-      </c>
-      <c r="C38" s="184" t="str">
+        <v>170</v>
+      </c>
+      <c r="C38" s="186" t="str">
         <f>VLOOKUP(B38,$B$50:$D$66,2,0)</f>
         <v>22 2752 8219</v>
       </c>
-      <c r="D38" s="184"/>
-      <c r="E38" s="184" t="str">
+      <c r="D38" s="186"/>
+      <c r="E38" s="186" t="str">
         <f>VLOOKUP(B38,$B$50:$D$66,3,0)</f>
         <v>jzepeda@qualtop.com</v>
       </c>
-      <c r="F38" s="184"/>
+      <c r="F38" s="186"/>
       <c r="G38" s="163" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="24.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A39" s="153"/>
       <c r="B39" s="154" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C39" s="154"/>
       <c r="D39" s="154"/>
@@ -5358,62 +5358,62 @@
     <row r="40" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A40" s="26"/>
       <c r="B40" s="21" t="s">
-        <v>164</v>
-      </c>
-      <c r="C40" s="184" t="str">
+        <v>163</v>
+      </c>
+      <c r="C40" s="186" t="str">
         <f>VLOOKUP(B40,$B$50:$D$66,2,0)</f>
         <v>33 1862 1719</v>
       </c>
-      <c r="D40" s="184"/>
-      <c r="E40" s="184" t="str">
+      <c r="D40" s="186"/>
+      <c r="E40" s="186" t="str">
         <f>VLOOKUP(B40,$B$50:$D$66,3,0)</f>
         <v>rpulido@qualtop.com</v>
       </c>
-      <c r="F40" s="184"/>
+      <c r="F40" s="186"/>
       <c r="G40" s="163" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A41" s="26"/>
       <c r="B41" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="C41" s="184" t="str">
+        <v>168</v>
+      </c>
+      <c r="C41" s="186" t="str">
         <f>VLOOKUP(B41,$B$50:$D$66,2,0)</f>
         <v>33 3504 5902</v>
       </c>
-      <c r="D41" s="184"/>
-      <c r="E41" s="184" t="str">
+      <c r="D41" s="186"/>
+      <c r="E41" s="186" t="str">
         <f>VLOOKUP(B41,$B$50:$D$66,3,0)</f>
         <v>charles.gonher@gmail.com</v>
       </c>
-      <c r="F41" s="184"/>
+      <c r="F41" s="186"/>
       <c r="G41" s="163" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A42" s="26"/>
       <c r="B42" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="C42" s="184" t="e">
+        <v>74</v>
+      </c>
+      <c r="C42" s="186" t="e">
         <f>VLOOKUP(B42,$B$50:$D$66,2,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="D42" s="184"/>
-      <c r="E42" s="184" t="e">
+      <c r="D42" s="186"/>
+      <c r="E42" s="186" t="e">
         <f>VLOOKUP(B42,$B$50:$D$66,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="F42" s="184"/>
+      <c r="F42" s="186"/>
       <c r="G42" s="23"/>
     </row>
     <row r="43" spans="1:7" ht="18.75" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A43" s="146"/>
       <c r="B43" s="145" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C43" s="146"/>
       <c r="D43" s="146"/>
@@ -5423,21 +5423,21 @@
     </row>
     <row r="44" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A44" s="5"/>
-      <c r="B44" s="198" t="s">
-        <v>242</v>
-      </c>
-      <c r="C44" s="188"/>
-      <c r="D44" s="188"/>
-      <c r="E44" s="188"/>
-      <c r="F44" s="188"/>
+      <c r="B44" s="184" t="s">
+        <v>241</v>
+      </c>
+      <c r="C44" s="185"/>
+      <c r="D44" s="185"/>
+      <c r="E44" s="185"/>
+      <c r="F44" s="185"/>
       <c r="G44" s="3"/>
     </row>
     <row r="45" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="188"/>
-      <c r="C45" s="188"/>
-      <c r="D45" s="188"/>
-      <c r="E45" s="188"/>
-      <c r="F45" s="188"/>
+      <c r="B45" s="185"/>
+      <c r="C45" s="185"/>
+      <c r="D45" s="185"/>
+      <c r="E45" s="185"/>
+      <c r="F45" s="185"/>
       <c r="G45" s="81"/>
     </row>
     <row r="46" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -5450,65 +5450,65 @@
         <v>0</v>
       </c>
       <c r="C49" s="89" t="s">
+        <v>15</v>
+      </c>
+      <c r="D49" s="89" t="s">
         <v>16</v>
-      </c>
-      <c r="D49" s="89" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="50" spans="2:4" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B50" s="84" t="s">
+        <v>168</v>
+      </c>
+      <c r="C50" s="85" t="s">
+        <v>173</v>
+      </c>
+      <c r="D50" s="82" t="s">
         <v>169</v>
-      </c>
-      <c r="C50" s="85" t="s">
-        <v>174</v>
-      </c>
-      <c r="D50" s="82" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="51" spans="2:4" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B51" s="84" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C51" s="85" t="s">
+        <v>174</v>
+      </c>
+      <c r="D51" s="82" t="s">
         <v>175</v>
-      </c>
-      <c r="D51" s="82" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="52" spans="2:4" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B52" s="84" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C52" s="85" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D52" s="82" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="53" spans="2:4" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B53" s="84" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C53" s="85" t="s">
+        <v>176</v>
+      </c>
+      <c r="D53" s="82" t="s">
         <v>177</v>
-      </c>
-      <c r="D53" s="82" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="54" spans="2:4" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B54" s="84" t="s">
+        <v>178</v>
+      </c>
+      <c r="C54" s="85" t="s">
         <v>179</v>
       </c>
-      <c r="C54" s="85" t="s">
+      <c r="D54" s="82" t="s">
         <v>180</v>
-      </c>
-      <c r="D54" s="82" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="55" spans="2:4" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -5574,6 +5574,33 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="43">
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E15:F15"/>
     <mergeCell ref="B44:F45"/>
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="E21:F21"/>
@@ -5590,33 +5617,6 @@
     <mergeCell ref="C41:D41"/>
     <mergeCell ref="E41:F41"/>
     <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E14:F14"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="WVM983093:WVM983106 JA50:JA66 SW50:SW66 ACS50:ACS66 AMO50:AMO66 AWK50:AWK66 BGG50:BGG66 BQC50:BQC66 BZY50:BZY66 CJU50:CJU66 CTQ50:CTQ66 DDM50:DDM66 DNI50:DNI66 DXE50:DXE66 EHA50:EHA66 EQW50:EQW66 FAS50:FAS66 FKO50:FKO66 FUK50:FUK66 GEG50:GEG66 GOC50:GOC66 GXY50:GXY66 HHU50:HHU66 HRQ50:HRQ66 IBM50:IBM66 ILI50:ILI66 IVE50:IVE66 JFA50:JFA66 JOW50:JOW66 JYS50:JYS66 KIO50:KIO66 KSK50:KSK66 LCG50:LCG66 LMC50:LMC66 LVY50:LVY66 MFU50:MFU66 MPQ50:MPQ66 MZM50:MZM66 NJI50:NJI66 NTE50:NTE66 ODA50:ODA66 OMW50:OMW66 OWS50:OWS66 PGO50:PGO66 PQK50:PQK66 QAG50:QAG66 QKC50:QKC66 QTY50:QTY66 RDU50:RDU66 RNQ50:RNQ66 RXM50:RXM66 SHI50:SHI66 SRE50:SRE66 TBA50:TBA66 TKW50:TKW66 TUS50:TUS66 UEO50:UEO66 UOK50:UOK66 UYG50:UYG66 VIC50:VIC66 VRY50:VRY66 WBU50:WBU66 WLQ50:WLQ66 WVM50:WVM66 D65570:D65583 JA65589:JA65602 SW65589:SW65602 ACS65589:ACS65602 AMO65589:AMO65602 AWK65589:AWK65602 BGG65589:BGG65602 BQC65589:BQC65602 BZY65589:BZY65602 CJU65589:CJU65602 CTQ65589:CTQ65602 DDM65589:DDM65602 DNI65589:DNI65602 DXE65589:DXE65602 EHA65589:EHA65602 EQW65589:EQW65602 FAS65589:FAS65602 FKO65589:FKO65602 FUK65589:FUK65602 GEG65589:GEG65602 GOC65589:GOC65602 GXY65589:GXY65602 HHU65589:HHU65602 HRQ65589:HRQ65602 IBM65589:IBM65602 ILI65589:ILI65602 IVE65589:IVE65602 JFA65589:JFA65602 JOW65589:JOW65602 JYS65589:JYS65602 KIO65589:KIO65602 KSK65589:KSK65602 LCG65589:LCG65602 LMC65589:LMC65602 LVY65589:LVY65602 MFU65589:MFU65602 MPQ65589:MPQ65602 MZM65589:MZM65602 NJI65589:NJI65602 NTE65589:NTE65602 ODA65589:ODA65602 OMW65589:OMW65602 OWS65589:OWS65602 PGO65589:PGO65602 PQK65589:PQK65602 QAG65589:QAG65602 QKC65589:QKC65602 QTY65589:QTY65602 RDU65589:RDU65602 RNQ65589:RNQ65602 RXM65589:RXM65602 SHI65589:SHI65602 SRE65589:SRE65602 TBA65589:TBA65602 TKW65589:TKW65602 TUS65589:TUS65602 UEO65589:UEO65602 UOK65589:UOK65602 UYG65589:UYG65602 VIC65589:VIC65602 VRY65589:VRY65602 WBU65589:WBU65602 WLQ65589:WLQ65602 WVM65589:WVM65602 D131106:D131119 JA131125:JA131138 SW131125:SW131138 ACS131125:ACS131138 AMO131125:AMO131138 AWK131125:AWK131138 BGG131125:BGG131138 BQC131125:BQC131138 BZY131125:BZY131138 CJU131125:CJU131138 CTQ131125:CTQ131138 DDM131125:DDM131138 DNI131125:DNI131138 DXE131125:DXE131138 EHA131125:EHA131138 EQW131125:EQW131138 FAS131125:FAS131138 FKO131125:FKO131138 FUK131125:FUK131138 GEG131125:GEG131138 GOC131125:GOC131138 GXY131125:GXY131138 HHU131125:HHU131138 HRQ131125:HRQ131138 IBM131125:IBM131138 ILI131125:ILI131138 IVE131125:IVE131138 JFA131125:JFA131138 JOW131125:JOW131138 JYS131125:JYS131138 KIO131125:KIO131138 KSK131125:KSK131138 LCG131125:LCG131138 LMC131125:LMC131138 LVY131125:LVY131138 MFU131125:MFU131138 MPQ131125:MPQ131138 MZM131125:MZM131138 NJI131125:NJI131138 NTE131125:NTE131138 ODA131125:ODA131138 OMW131125:OMW131138 OWS131125:OWS131138 PGO131125:PGO131138 PQK131125:PQK131138 QAG131125:QAG131138 QKC131125:QKC131138 QTY131125:QTY131138 RDU131125:RDU131138 RNQ131125:RNQ131138 RXM131125:RXM131138 SHI131125:SHI131138 SRE131125:SRE131138 TBA131125:TBA131138 TKW131125:TKW131138 TUS131125:TUS131138 UEO131125:UEO131138 UOK131125:UOK131138 UYG131125:UYG131138 VIC131125:VIC131138 VRY131125:VRY131138 WBU131125:WBU131138 WLQ131125:WLQ131138 WVM131125:WVM131138 D196642:D196655 JA196661:JA196674 SW196661:SW196674 ACS196661:ACS196674 AMO196661:AMO196674 AWK196661:AWK196674 BGG196661:BGG196674 BQC196661:BQC196674 BZY196661:BZY196674 CJU196661:CJU196674 CTQ196661:CTQ196674 DDM196661:DDM196674 DNI196661:DNI196674 DXE196661:DXE196674 EHA196661:EHA196674 EQW196661:EQW196674 FAS196661:FAS196674 FKO196661:FKO196674 FUK196661:FUK196674 GEG196661:GEG196674 GOC196661:GOC196674 GXY196661:GXY196674 HHU196661:HHU196674 HRQ196661:HRQ196674 IBM196661:IBM196674 ILI196661:ILI196674 IVE196661:IVE196674 JFA196661:JFA196674 JOW196661:JOW196674 JYS196661:JYS196674 KIO196661:KIO196674 KSK196661:KSK196674 LCG196661:LCG196674 LMC196661:LMC196674 LVY196661:LVY196674 MFU196661:MFU196674 MPQ196661:MPQ196674 MZM196661:MZM196674 NJI196661:NJI196674 NTE196661:NTE196674 ODA196661:ODA196674 OMW196661:OMW196674 OWS196661:OWS196674 PGO196661:PGO196674 PQK196661:PQK196674 QAG196661:QAG196674 QKC196661:QKC196674 QTY196661:QTY196674 RDU196661:RDU196674 RNQ196661:RNQ196674 RXM196661:RXM196674 SHI196661:SHI196674 SRE196661:SRE196674 TBA196661:TBA196674 TKW196661:TKW196674 TUS196661:TUS196674 UEO196661:UEO196674 UOK196661:UOK196674 UYG196661:UYG196674 VIC196661:VIC196674 VRY196661:VRY196674 WBU196661:WBU196674 WLQ196661:WLQ196674 WVM196661:WVM196674 D262178:D262191 JA262197:JA262210 SW262197:SW262210 ACS262197:ACS262210 AMO262197:AMO262210 AWK262197:AWK262210 BGG262197:BGG262210 BQC262197:BQC262210 BZY262197:BZY262210 CJU262197:CJU262210 CTQ262197:CTQ262210 DDM262197:DDM262210 DNI262197:DNI262210 DXE262197:DXE262210 EHA262197:EHA262210 EQW262197:EQW262210 FAS262197:FAS262210 FKO262197:FKO262210 FUK262197:FUK262210 GEG262197:GEG262210 GOC262197:GOC262210 GXY262197:GXY262210 HHU262197:HHU262210 HRQ262197:HRQ262210 IBM262197:IBM262210 ILI262197:ILI262210 IVE262197:IVE262210 JFA262197:JFA262210 JOW262197:JOW262210 JYS262197:JYS262210 KIO262197:KIO262210 KSK262197:KSK262210 LCG262197:LCG262210 LMC262197:LMC262210 LVY262197:LVY262210 MFU262197:MFU262210 MPQ262197:MPQ262210 MZM262197:MZM262210 NJI262197:NJI262210 NTE262197:NTE262210 ODA262197:ODA262210 OMW262197:OMW262210 OWS262197:OWS262210 PGO262197:PGO262210 PQK262197:PQK262210 QAG262197:QAG262210 QKC262197:QKC262210 QTY262197:QTY262210 RDU262197:RDU262210 RNQ262197:RNQ262210 RXM262197:RXM262210 SHI262197:SHI262210 SRE262197:SRE262210 TBA262197:TBA262210 TKW262197:TKW262210 TUS262197:TUS262210 UEO262197:UEO262210 UOK262197:UOK262210 UYG262197:UYG262210 VIC262197:VIC262210 VRY262197:VRY262210 WBU262197:WBU262210 WLQ262197:WLQ262210 WVM262197:WVM262210 D327714:D327727 JA327733:JA327746 SW327733:SW327746 ACS327733:ACS327746 AMO327733:AMO327746 AWK327733:AWK327746 BGG327733:BGG327746 BQC327733:BQC327746 BZY327733:BZY327746 CJU327733:CJU327746 CTQ327733:CTQ327746 DDM327733:DDM327746 DNI327733:DNI327746 DXE327733:DXE327746 EHA327733:EHA327746 EQW327733:EQW327746 FAS327733:FAS327746 FKO327733:FKO327746 FUK327733:FUK327746 GEG327733:GEG327746 GOC327733:GOC327746 GXY327733:GXY327746 HHU327733:HHU327746 HRQ327733:HRQ327746 IBM327733:IBM327746 ILI327733:ILI327746 IVE327733:IVE327746 JFA327733:JFA327746 JOW327733:JOW327746 JYS327733:JYS327746 KIO327733:KIO327746 KSK327733:KSK327746 LCG327733:LCG327746 LMC327733:LMC327746 LVY327733:LVY327746 MFU327733:MFU327746 MPQ327733:MPQ327746 MZM327733:MZM327746 NJI327733:NJI327746 NTE327733:NTE327746 ODA327733:ODA327746 OMW327733:OMW327746 OWS327733:OWS327746 PGO327733:PGO327746 PQK327733:PQK327746 QAG327733:QAG327746 QKC327733:QKC327746 QTY327733:QTY327746 RDU327733:RDU327746 RNQ327733:RNQ327746 RXM327733:RXM327746 SHI327733:SHI327746 SRE327733:SRE327746 TBA327733:TBA327746 TKW327733:TKW327746 TUS327733:TUS327746 UEO327733:UEO327746 UOK327733:UOK327746 UYG327733:UYG327746 VIC327733:VIC327746 VRY327733:VRY327746 WBU327733:WBU327746 WLQ327733:WLQ327746 WVM327733:WVM327746 D393250:D393263 JA393269:JA393282 SW393269:SW393282 ACS393269:ACS393282 AMO393269:AMO393282 AWK393269:AWK393282 BGG393269:BGG393282 BQC393269:BQC393282 BZY393269:BZY393282 CJU393269:CJU393282 CTQ393269:CTQ393282 DDM393269:DDM393282 DNI393269:DNI393282 DXE393269:DXE393282 EHA393269:EHA393282 EQW393269:EQW393282 FAS393269:FAS393282 FKO393269:FKO393282 FUK393269:FUK393282 GEG393269:GEG393282 GOC393269:GOC393282 GXY393269:GXY393282 HHU393269:HHU393282 HRQ393269:HRQ393282 IBM393269:IBM393282 ILI393269:ILI393282 IVE393269:IVE393282 JFA393269:JFA393282 JOW393269:JOW393282 JYS393269:JYS393282 KIO393269:KIO393282 KSK393269:KSK393282 LCG393269:LCG393282 LMC393269:LMC393282 LVY393269:LVY393282 MFU393269:MFU393282 MPQ393269:MPQ393282 MZM393269:MZM393282 NJI393269:NJI393282 NTE393269:NTE393282 ODA393269:ODA393282 OMW393269:OMW393282 OWS393269:OWS393282 PGO393269:PGO393282 PQK393269:PQK393282 QAG393269:QAG393282 QKC393269:QKC393282 QTY393269:QTY393282 RDU393269:RDU393282 RNQ393269:RNQ393282 RXM393269:RXM393282 SHI393269:SHI393282 SRE393269:SRE393282 TBA393269:TBA393282 TKW393269:TKW393282 TUS393269:TUS393282 UEO393269:UEO393282 UOK393269:UOK393282 UYG393269:UYG393282 VIC393269:VIC393282 VRY393269:VRY393282 WBU393269:WBU393282 WLQ393269:WLQ393282 WVM393269:WVM393282 D458786:D458799 JA458805:JA458818 SW458805:SW458818 ACS458805:ACS458818 AMO458805:AMO458818 AWK458805:AWK458818 BGG458805:BGG458818 BQC458805:BQC458818 BZY458805:BZY458818 CJU458805:CJU458818 CTQ458805:CTQ458818 DDM458805:DDM458818 DNI458805:DNI458818 DXE458805:DXE458818 EHA458805:EHA458818 EQW458805:EQW458818 FAS458805:FAS458818 FKO458805:FKO458818 FUK458805:FUK458818 GEG458805:GEG458818 GOC458805:GOC458818 GXY458805:GXY458818 HHU458805:HHU458818 HRQ458805:HRQ458818 IBM458805:IBM458818 ILI458805:ILI458818 IVE458805:IVE458818 JFA458805:JFA458818 JOW458805:JOW458818 JYS458805:JYS458818 KIO458805:KIO458818 KSK458805:KSK458818 LCG458805:LCG458818 LMC458805:LMC458818 LVY458805:LVY458818 MFU458805:MFU458818 MPQ458805:MPQ458818 MZM458805:MZM458818 NJI458805:NJI458818 NTE458805:NTE458818 ODA458805:ODA458818 OMW458805:OMW458818 OWS458805:OWS458818 PGO458805:PGO458818 PQK458805:PQK458818 QAG458805:QAG458818 QKC458805:QKC458818 QTY458805:QTY458818 RDU458805:RDU458818 RNQ458805:RNQ458818 RXM458805:RXM458818 SHI458805:SHI458818 SRE458805:SRE458818 TBA458805:TBA458818 TKW458805:TKW458818 TUS458805:TUS458818 UEO458805:UEO458818 UOK458805:UOK458818 UYG458805:UYG458818 VIC458805:VIC458818 VRY458805:VRY458818 WBU458805:WBU458818 WLQ458805:WLQ458818 WVM458805:WVM458818 D524322:D524335 JA524341:JA524354 SW524341:SW524354 ACS524341:ACS524354 AMO524341:AMO524354 AWK524341:AWK524354 BGG524341:BGG524354 BQC524341:BQC524354 BZY524341:BZY524354 CJU524341:CJU524354 CTQ524341:CTQ524354 DDM524341:DDM524354 DNI524341:DNI524354 DXE524341:DXE524354 EHA524341:EHA524354 EQW524341:EQW524354 FAS524341:FAS524354 FKO524341:FKO524354 FUK524341:FUK524354 GEG524341:GEG524354 GOC524341:GOC524354 GXY524341:GXY524354 HHU524341:HHU524354 HRQ524341:HRQ524354 IBM524341:IBM524354 ILI524341:ILI524354 IVE524341:IVE524354 JFA524341:JFA524354 JOW524341:JOW524354 JYS524341:JYS524354 KIO524341:KIO524354 KSK524341:KSK524354 LCG524341:LCG524354 LMC524341:LMC524354 LVY524341:LVY524354 MFU524341:MFU524354 MPQ524341:MPQ524354 MZM524341:MZM524354 NJI524341:NJI524354 NTE524341:NTE524354 ODA524341:ODA524354 OMW524341:OMW524354 OWS524341:OWS524354 PGO524341:PGO524354 PQK524341:PQK524354 QAG524341:QAG524354 QKC524341:QKC524354 QTY524341:QTY524354 RDU524341:RDU524354 RNQ524341:RNQ524354 RXM524341:RXM524354 SHI524341:SHI524354 SRE524341:SRE524354 TBA524341:TBA524354 TKW524341:TKW524354 TUS524341:TUS524354 UEO524341:UEO524354 UOK524341:UOK524354 UYG524341:UYG524354 VIC524341:VIC524354 VRY524341:VRY524354 WBU524341:WBU524354 WLQ524341:WLQ524354 WVM524341:WVM524354 D589858:D589871 JA589877:JA589890 SW589877:SW589890 ACS589877:ACS589890 AMO589877:AMO589890 AWK589877:AWK589890 BGG589877:BGG589890 BQC589877:BQC589890 BZY589877:BZY589890 CJU589877:CJU589890 CTQ589877:CTQ589890 DDM589877:DDM589890 DNI589877:DNI589890 DXE589877:DXE589890 EHA589877:EHA589890 EQW589877:EQW589890 FAS589877:FAS589890 FKO589877:FKO589890 FUK589877:FUK589890 GEG589877:GEG589890 GOC589877:GOC589890 GXY589877:GXY589890 HHU589877:HHU589890 HRQ589877:HRQ589890 IBM589877:IBM589890 ILI589877:ILI589890 IVE589877:IVE589890 JFA589877:JFA589890 JOW589877:JOW589890 JYS589877:JYS589890 KIO589877:KIO589890 KSK589877:KSK589890 LCG589877:LCG589890 LMC589877:LMC589890 LVY589877:LVY589890 MFU589877:MFU589890 MPQ589877:MPQ589890 MZM589877:MZM589890 NJI589877:NJI589890 NTE589877:NTE589890 ODA589877:ODA589890 OMW589877:OMW589890 OWS589877:OWS589890 PGO589877:PGO589890 PQK589877:PQK589890 QAG589877:QAG589890 QKC589877:QKC589890 QTY589877:QTY589890 RDU589877:RDU589890 RNQ589877:RNQ589890 RXM589877:RXM589890 SHI589877:SHI589890 SRE589877:SRE589890 TBA589877:TBA589890 TKW589877:TKW589890 TUS589877:TUS589890 UEO589877:UEO589890 UOK589877:UOK589890 UYG589877:UYG589890 VIC589877:VIC589890 VRY589877:VRY589890 WBU589877:WBU589890 WLQ589877:WLQ589890 WVM589877:WVM589890 D655394:D655407 JA655413:JA655426 SW655413:SW655426 ACS655413:ACS655426 AMO655413:AMO655426 AWK655413:AWK655426 BGG655413:BGG655426 BQC655413:BQC655426 BZY655413:BZY655426 CJU655413:CJU655426 CTQ655413:CTQ655426 DDM655413:DDM655426 DNI655413:DNI655426 DXE655413:DXE655426 EHA655413:EHA655426 EQW655413:EQW655426 FAS655413:FAS655426 FKO655413:FKO655426 FUK655413:FUK655426 GEG655413:GEG655426 GOC655413:GOC655426 GXY655413:GXY655426 HHU655413:HHU655426 HRQ655413:HRQ655426 IBM655413:IBM655426 ILI655413:ILI655426 IVE655413:IVE655426 JFA655413:JFA655426 JOW655413:JOW655426 JYS655413:JYS655426 KIO655413:KIO655426 KSK655413:KSK655426 LCG655413:LCG655426 LMC655413:LMC655426 LVY655413:LVY655426 MFU655413:MFU655426 MPQ655413:MPQ655426 MZM655413:MZM655426 NJI655413:NJI655426 NTE655413:NTE655426 ODA655413:ODA655426 OMW655413:OMW655426 OWS655413:OWS655426 PGO655413:PGO655426 PQK655413:PQK655426 QAG655413:QAG655426 QKC655413:QKC655426 QTY655413:QTY655426 RDU655413:RDU655426 RNQ655413:RNQ655426 RXM655413:RXM655426 SHI655413:SHI655426 SRE655413:SRE655426 TBA655413:TBA655426 TKW655413:TKW655426 TUS655413:TUS655426 UEO655413:UEO655426 UOK655413:UOK655426 UYG655413:UYG655426 VIC655413:VIC655426 VRY655413:VRY655426 WBU655413:WBU655426 WLQ655413:WLQ655426 WVM655413:WVM655426 D720930:D720943 JA720949:JA720962 SW720949:SW720962 ACS720949:ACS720962 AMO720949:AMO720962 AWK720949:AWK720962 BGG720949:BGG720962 BQC720949:BQC720962 BZY720949:BZY720962 CJU720949:CJU720962 CTQ720949:CTQ720962 DDM720949:DDM720962 DNI720949:DNI720962 DXE720949:DXE720962 EHA720949:EHA720962 EQW720949:EQW720962 FAS720949:FAS720962 FKO720949:FKO720962 FUK720949:FUK720962 GEG720949:GEG720962 GOC720949:GOC720962 GXY720949:GXY720962 HHU720949:HHU720962 HRQ720949:HRQ720962 IBM720949:IBM720962 ILI720949:ILI720962 IVE720949:IVE720962 JFA720949:JFA720962 JOW720949:JOW720962 JYS720949:JYS720962 KIO720949:KIO720962 KSK720949:KSK720962 LCG720949:LCG720962 LMC720949:LMC720962 LVY720949:LVY720962 MFU720949:MFU720962 MPQ720949:MPQ720962 MZM720949:MZM720962 NJI720949:NJI720962 NTE720949:NTE720962 ODA720949:ODA720962 OMW720949:OMW720962 OWS720949:OWS720962 PGO720949:PGO720962 PQK720949:PQK720962 QAG720949:QAG720962 QKC720949:QKC720962 QTY720949:QTY720962 RDU720949:RDU720962 RNQ720949:RNQ720962 RXM720949:RXM720962 SHI720949:SHI720962 SRE720949:SRE720962 TBA720949:TBA720962 TKW720949:TKW720962 TUS720949:TUS720962 UEO720949:UEO720962 UOK720949:UOK720962 UYG720949:UYG720962 VIC720949:VIC720962 VRY720949:VRY720962 WBU720949:WBU720962 WLQ720949:WLQ720962 WVM720949:WVM720962 D786466:D786479 JA786485:JA786498 SW786485:SW786498 ACS786485:ACS786498 AMO786485:AMO786498 AWK786485:AWK786498 BGG786485:BGG786498 BQC786485:BQC786498 BZY786485:BZY786498 CJU786485:CJU786498 CTQ786485:CTQ786498 DDM786485:DDM786498 DNI786485:DNI786498 DXE786485:DXE786498 EHA786485:EHA786498 EQW786485:EQW786498 FAS786485:FAS786498 FKO786485:FKO786498 FUK786485:FUK786498 GEG786485:GEG786498 GOC786485:GOC786498 GXY786485:GXY786498 HHU786485:HHU786498 HRQ786485:HRQ786498 IBM786485:IBM786498 ILI786485:ILI786498 IVE786485:IVE786498 JFA786485:JFA786498 JOW786485:JOW786498 JYS786485:JYS786498 KIO786485:KIO786498 KSK786485:KSK786498 LCG786485:LCG786498 LMC786485:LMC786498 LVY786485:LVY786498 MFU786485:MFU786498 MPQ786485:MPQ786498 MZM786485:MZM786498 NJI786485:NJI786498 NTE786485:NTE786498 ODA786485:ODA786498 OMW786485:OMW786498 OWS786485:OWS786498 PGO786485:PGO786498 PQK786485:PQK786498 QAG786485:QAG786498 QKC786485:QKC786498 QTY786485:QTY786498 RDU786485:RDU786498 RNQ786485:RNQ786498 RXM786485:RXM786498 SHI786485:SHI786498 SRE786485:SRE786498 TBA786485:TBA786498 TKW786485:TKW786498 TUS786485:TUS786498 UEO786485:UEO786498 UOK786485:UOK786498 UYG786485:UYG786498 VIC786485:VIC786498 VRY786485:VRY786498 WBU786485:WBU786498 WLQ786485:WLQ786498 WVM786485:WVM786498 D852002:D852015 JA852021:JA852034 SW852021:SW852034 ACS852021:ACS852034 AMO852021:AMO852034 AWK852021:AWK852034 BGG852021:BGG852034 BQC852021:BQC852034 BZY852021:BZY852034 CJU852021:CJU852034 CTQ852021:CTQ852034 DDM852021:DDM852034 DNI852021:DNI852034 DXE852021:DXE852034 EHA852021:EHA852034 EQW852021:EQW852034 FAS852021:FAS852034 FKO852021:FKO852034 FUK852021:FUK852034 GEG852021:GEG852034 GOC852021:GOC852034 GXY852021:GXY852034 HHU852021:HHU852034 HRQ852021:HRQ852034 IBM852021:IBM852034 ILI852021:ILI852034 IVE852021:IVE852034 JFA852021:JFA852034 JOW852021:JOW852034 JYS852021:JYS852034 KIO852021:KIO852034 KSK852021:KSK852034 LCG852021:LCG852034 LMC852021:LMC852034 LVY852021:LVY852034 MFU852021:MFU852034 MPQ852021:MPQ852034 MZM852021:MZM852034 NJI852021:NJI852034 NTE852021:NTE852034 ODA852021:ODA852034 OMW852021:OMW852034 OWS852021:OWS852034 PGO852021:PGO852034 PQK852021:PQK852034 QAG852021:QAG852034 QKC852021:QKC852034 QTY852021:QTY852034 RDU852021:RDU852034 RNQ852021:RNQ852034 RXM852021:RXM852034 SHI852021:SHI852034 SRE852021:SRE852034 TBA852021:TBA852034 TKW852021:TKW852034 TUS852021:TUS852034 UEO852021:UEO852034 UOK852021:UOK852034 UYG852021:UYG852034 VIC852021:VIC852034 VRY852021:VRY852034 WBU852021:WBU852034 WLQ852021:WLQ852034 WVM852021:WVM852034 D917538:D917551 JA917557:JA917570 SW917557:SW917570 ACS917557:ACS917570 AMO917557:AMO917570 AWK917557:AWK917570 BGG917557:BGG917570 BQC917557:BQC917570 BZY917557:BZY917570 CJU917557:CJU917570 CTQ917557:CTQ917570 DDM917557:DDM917570 DNI917557:DNI917570 DXE917557:DXE917570 EHA917557:EHA917570 EQW917557:EQW917570 FAS917557:FAS917570 FKO917557:FKO917570 FUK917557:FUK917570 GEG917557:GEG917570 GOC917557:GOC917570 GXY917557:GXY917570 HHU917557:HHU917570 HRQ917557:HRQ917570 IBM917557:IBM917570 ILI917557:ILI917570 IVE917557:IVE917570 JFA917557:JFA917570 JOW917557:JOW917570 JYS917557:JYS917570 KIO917557:KIO917570 KSK917557:KSK917570 LCG917557:LCG917570 LMC917557:LMC917570 LVY917557:LVY917570 MFU917557:MFU917570 MPQ917557:MPQ917570 MZM917557:MZM917570 NJI917557:NJI917570 NTE917557:NTE917570 ODA917557:ODA917570 OMW917557:OMW917570 OWS917557:OWS917570 PGO917557:PGO917570 PQK917557:PQK917570 QAG917557:QAG917570 QKC917557:QKC917570 QTY917557:QTY917570 RDU917557:RDU917570 RNQ917557:RNQ917570 RXM917557:RXM917570 SHI917557:SHI917570 SRE917557:SRE917570 TBA917557:TBA917570 TKW917557:TKW917570 TUS917557:TUS917570 UEO917557:UEO917570 UOK917557:UOK917570 UYG917557:UYG917570 VIC917557:VIC917570 VRY917557:VRY917570 WBU917557:WBU917570 WLQ917557:WLQ917570 WVM917557:WVM917570 D983074:D983087 JA983093:JA983106 SW983093:SW983106 ACS983093:ACS983106 AMO983093:AMO983106 AWK983093:AWK983106 BGG983093:BGG983106 BQC983093:BQC983106 BZY983093:BZY983106 CJU983093:CJU983106 CTQ983093:CTQ983106 DDM983093:DDM983106 DNI983093:DNI983106 DXE983093:DXE983106 EHA983093:EHA983106 EQW983093:EQW983106 FAS983093:FAS983106 FKO983093:FKO983106 FUK983093:FUK983106 GEG983093:GEG983106 GOC983093:GOC983106 GXY983093:GXY983106 HHU983093:HHU983106 HRQ983093:HRQ983106 IBM983093:IBM983106 ILI983093:ILI983106 IVE983093:IVE983106 JFA983093:JFA983106 JOW983093:JOW983106 JYS983093:JYS983106 KIO983093:KIO983106 KSK983093:KSK983106 LCG983093:LCG983106 LMC983093:LMC983106 LVY983093:LVY983106 MFU983093:MFU983106 MPQ983093:MPQ983106 MZM983093:MZM983106 NJI983093:NJI983106 NTE983093:NTE983106 ODA983093:ODA983106 OMW983093:OMW983106 OWS983093:OWS983106 PGO983093:PGO983106 PQK983093:PQK983106 QAG983093:QAG983106 QKC983093:QKC983106 QTY983093:QTY983106 RDU983093:RDU983106 RNQ983093:RNQ983106 RXM983093:RXM983106 SHI983093:SHI983106 SRE983093:SRE983106 TBA983093:TBA983106 TKW983093:TKW983106 TUS983093:TUS983106 UEO983093:UEO983106 UOK983093:UOK983106 UYG983093:UYG983106 VIC983093:VIC983106 VRY983093:VRY983106 WBU983093:WBU983106 WLQ983093:WLQ983106">
@@ -6453,7 +6453,7 @@
     <row r="2" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="148"/>
       <c r="B2" s="149" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C2" s="148"/>
       <c r="D2" s="148"/>
@@ -6464,77 +6464,77 @@
     <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="7" t="s">
+      <c r="F3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>18</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="127.5" x14ac:dyDescent="0.2">
       <c r="A4" s="10"/>
       <c r="B4" s="11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C4" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="D4" s="13" t="s">
         <v>254</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="E4" s="12" t="s">
         <v>255</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="F4" s="12" t="s">
         <v>256</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>257</v>
       </c>
       <c r="G4" s="12"/>
     </row>
     <row r="5" spans="1:12" s="10" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="B5" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="E5" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="C5" s="12" t="s">
-        <v>254</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>222</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>184</v>
-      </c>
       <c r="F5" s="12" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G5" s="12"/>
       <c r="L5" s="82"/>
     </row>
     <row r="6" spans="1:12" s="10" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B6" s="11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E6" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="F6" s="12" t="s">
         <v>223</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>224</v>
       </c>
       <c r="G6" s="12"/>
       <c r="L6" s="82"/>
@@ -7603,7 +7603,7 @@
     <row r="2" spans="1:269" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="132"/>
       <c r="B2" s="133" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C2" s="133"/>
       <c r="D2" s="132"/>
@@ -7621,11 +7621,11 @@
       <c r="P2" s="132"/>
       <c r="Q2" s="132"/>
       <c r="R2" s="132"/>
-      <c r="S2" s="189" t="s">
-        <v>47</v>
+      <c r="S2" s="190" t="s">
+        <v>46</v>
       </c>
       <c r="JB2" s="160" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="JC2" s="27">
         <v>5</v>
@@ -7649,60 +7649,60 @@
     </row>
     <row r="3" spans="1:269" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" s="38" t="s">
+        <v>100</v>
+      </c>
+      <c r="G3" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="H3" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="I3" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="38" t="s">
-        <v>61</v>
-      </c>
-      <c r="C3" s="38" t="s">
-        <v>62</v>
-      </c>
-      <c r="D3" s="38" t="s">
-        <v>63</v>
-      </c>
-      <c r="E3" s="38" t="s">
-        <v>59</v>
-      </c>
-      <c r="F3" s="38" t="s">
-        <v>101</v>
-      </c>
-      <c r="G3" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="H3" s="38" t="s">
-        <v>47</v>
-      </c>
-      <c r="I3" s="38" t="s">
-        <v>36</v>
-      </c>
       <c r="J3" s="38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K3" s="37"/>
       <c r="L3" s="57" t="s">
+        <v>57</v>
+      </c>
+      <c r="M3" s="57" t="s">
+        <v>56</v>
+      </c>
+      <c r="N3" s="38" t="s">
+        <v>262</v>
+      </c>
+      <c r="O3" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="P3" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q3" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="M3" s="57" t="s">
-        <v>57</v>
-      </c>
-      <c r="N3" s="38" t="s">
-        <v>263</v>
-      </c>
-      <c r="O3" s="38" t="s">
-        <v>56</v>
-      </c>
-      <c r="P3" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q3" s="38" t="s">
-        <v>59</v>
-      </c>
       <c r="R3" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="S3" s="189"/>
+        <v>10</v>
+      </c>
+      <c r="S3" s="190"/>
       <c r="JB3" s="160" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="JC3" s="27">
         <v>4</v>
@@ -7727,7 +7727,7 @@
     <row r="4" spans="1:269" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="165"/>
       <c r="B4" s="164" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C4" s="164"/>
       <c r="D4" s="166"/>
@@ -7745,9 +7745,9 @@
       <c r="P4" s="170"/>
       <c r="Q4" s="170"/>
       <c r="R4" s="169"/>
-      <c r="S4" s="189"/>
+      <c r="S4" s="190"/>
       <c r="JB4" s="160" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="JC4" s="27">
         <v>3</v>
@@ -7774,19 +7774,19 @@
         <v>1</v>
       </c>
       <c r="B5" s="54" t="s">
+        <v>263</v>
+      </c>
+      <c r="C5" s="54" t="s">
         <v>264</v>
       </c>
-      <c r="C5" s="54" t="s">
-        <v>265</v>
-      </c>
       <c r="D5" s="73" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E5" s="56" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F5" s="56" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G5" s="141">
         <v>1</v>
@@ -7795,32 +7795,32 @@
         <v>3</v>
       </c>
       <c r="I5" s="138" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" s="137" t="s">
         <v>38</v>
-      </c>
-      <c r="J5" s="137" t="s">
-        <v>39</v>
       </c>
       <c r="K5" s="35"/>
       <c r="L5" s="54" t="s">
+        <v>265</v>
+      </c>
+      <c r="M5" s="175" t="s">
         <v>266</v>
       </c>
-      <c r="M5" s="175" t="s">
-        <v>267</v>
-      </c>
       <c r="N5" s="175" t="s">
+        <v>202</v>
+      </c>
+      <c r="O5" s="52" t="s">
         <v>203</v>
       </c>
-      <c r="O5" s="52" t="s">
+      <c r="P5" s="52" t="s">
         <v>204</v>
       </c>
-      <c r="P5" s="52" t="s">
-        <v>205</v>
-      </c>
       <c r="Q5" s="52" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="R5" s="42"/>
-      <c r="S5" s="189"/>
+      <c r="S5" s="190"/>
       <c r="JB5" s="160"/>
       <c r="JD5" s="105"/>
       <c r="JE5" s="107"/>
@@ -7834,19 +7834,19 @@
         <v>2</v>
       </c>
       <c r="B6" s="53" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C6" s="54" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D6" s="73" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E6" s="56" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F6" s="56" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G6" s="141">
         <v>2</v>
@@ -7855,34 +7855,34 @@
         <v>1</v>
       </c>
       <c r="I6" s="139" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J6" s="137" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K6" s="35"/>
       <c r="L6" s="53" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="M6" s="175" t="s">
+        <v>268</v>
+      </c>
+      <c r="N6" s="175" t="s">
         <v>269</v>
       </c>
-      <c r="N6" s="175" t="s">
-        <v>270</v>
-      </c>
       <c r="O6" s="52" t="s">
+        <v>207</v>
+      </c>
+      <c r="P6" s="52" t="s">
         <v>208</v>
       </c>
-      <c r="P6" s="52" t="s">
-        <v>209</v>
-      </c>
       <c r="Q6" s="52" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="R6" s="59"/>
-      <c r="S6" s="189"/>
+      <c r="S6" s="190"/>
       <c r="JB6" s="160" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="JC6" s="27">
         <v>2</v>
@@ -7909,19 +7909,19 @@
         <v>3</v>
       </c>
       <c r="B7" s="53" t="s">
+        <v>184</v>
+      </c>
+      <c r="C7" s="54" t="s">
         <v>185</v>
       </c>
-      <c r="C7" s="54" t="s">
-        <v>186</v>
-      </c>
       <c r="D7" s="73" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E7" s="56" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F7" s="56" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G7" s="141">
         <v>2</v>
@@ -7930,34 +7930,34 @@
         <v>1</v>
       </c>
       <c r="I7" s="138" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J7" s="137" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K7" s="35"/>
       <c r="L7" s="53" t="s">
+        <v>270</v>
+      </c>
+      <c r="M7" s="175" t="s">
         <v>271</v>
       </c>
-      <c r="M7" s="175" t="s">
+      <c r="N7" s="175" t="s">
         <v>272</v>
       </c>
-      <c r="N7" s="175" t="s">
+      <c r="O7" s="52" t="s">
         <v>273</v>
       </c>
-      <c r="O7" s="52" t="s">
-        <v>274</v>
-      </c>
       <c r="P7" s="52" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="Q7" s="52" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="R7" s="59"/>
-      <c r="S7" s="189"/>
+      <c r="S7" s="190"/>
       <c r="JB7" s="160" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="JC7" s="27">
         <v>1</v>
@@ -7984,19 +7984,19 @@
         <v>4</v>
       </c>
       <c r="B8" s="53" t="s">
+        <v>186</v>
+      </c>
+      <c r="C8" s="54" t="s">
         <v>187</v>
       </c>
-      <c r="C8" s="54" t="s">
-        <v>188</v>
-      </c>
       <c r="D8" s="73" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E8" s="56" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F8" s="56" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G8" s="141">
         <v>1</v>
@@ -8005,29 +8005,29 @@
         <v>1</v>
       </c>
       <c r="I8" s="139" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J8" s="137" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K8" s="35"/>
       <c r="L8" s="53" t="s">
+        <v>274</v>
+      </c>
+      <c r="M8" s="175" t="s">
         <v>275</v>
       </c>
-      <c r="M8" s="175" t="s">
+      <c r="N8" s="175" t="s">
+        <v>211</v>
+      </c>
+      <c r="O8" s="52" t="s">
         <v>276</v>
       </c>
-      <c r="N8" s="175" t="s">
+      <c r="P8" s="52" t="s">
         <v>212</v>
       </c>
-      <c r="O8" s="52" t="s">
-        <v>277</v>
-      </c>
-      <c r="P8" s="52" t="s">
-        <v>213</v>
-      </c>
       <c r="Q8" s="52" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="R8" s="59"/>
       <c r="JC8" s="32"/>
@@ -8051,7 +8051,7 @@
     <row r="9" spans="1:269" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="171"/>
       <c r="B9" s="172" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C9" s="164"/>
       <c r="D9" s="166"/>
@@ -8071,19 +8071,19 @@
       <c r="R9" s="174"/>
       <c r="JC9" s="32"/>
       <c r="JD9" s="160" t="s">
+        <v>147</v>
+      </c>
+      <c r="JE9" s="160" t="s">
         <v>148</v>
       </c>
-      <c r="JE9" s="160" t="s">
+      <c r="JF9" s="160" t="s">
         <v>149</v>
       </c>
-      <c r="JF9" s="160" t="s">
-        <v>150</v>
-      </c>
       <c r="JG9" s="160" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="JH9" s="160" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="JI9" s="32"/>
     </row>
@@ -8092,19 +8092,19 @@
         <v>1</v>
       </c>
       <c r="B10" s="53" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C10" s="54" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D10" s="73" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E10" s="56" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F10" s="56" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G10" s="141">
         <v>1</v>
@@ -8113,35 +8113,35 @@
         <v>1</v>
       </c>
       <c r="I10" s="139" t="s">
+        <v>36</v>
+      </c>
+      <c r="J10" s="137" t="s">
         <v>37</v>
-      </c>
-      <c r="J10" s="137" t="s">
-        <v>38</v>
       </c>
       <c r="K10" s="35"/>
       <c r="L10" s="53" t="s">
+        <v>278</v>
+      </c>
+      <c r="M10" s="175" t="s">
         <v>279</v>
       </c>
-      <c r="M10" s="175" t="s">
+      <c r="N10" s="36" t="s">
+        <v>213</v>
+      </c>
+      <c r="O10" s="52" t="s">
         <v>280</v>
       </c>
-      <c r="N10" s="36" t="s">
-        <v>214</v>
-      </c>
-      <c r="O10" s="52" t="s">
-        <v>281</v>
-      </c>
       <c r="P10" s="52" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Q10" s="52" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="R10" s="59"/>
       <c r="JC10" s="32"/>
       <c r="JD10" s="32"/>
       <c r="JE10" s="160" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="JF10" s="34"/>
       <c r="JG10" s="34"/>
@@ -8153,19 +8153,19 @@
         <v>2</v>
       </c>
       <c r="B11" s="53" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C11" s="54" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D11" s="73" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E11" s="56" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F11" s="56" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G11" s="141">
         <v>2</v>
@@ -8174,29 +8174,29 @@
         <v>1</v>
       </c>
       <c r="I11" s="138" t="s">
+        <v>37</v>
+      </c>
+      <c r="J11" s="137" t="s">
         <v>38</v>
-      </c>
-      <c r="J11" s="137" t="s">
-        <v>39</v>
       </c>
       <c r="K11" s="35"/>
       <c r="L11" s="53" t="s">
+        <v>214</v>
+      </c>
+      <c r="M11" s="175" t="s">
         <v>215</v>
       </c>
-      <c r="M11" s="175" t="s">
-        <v>216</v>
-      </c>
       <c r="N11" s="175" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="O11" s="52" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="P11" s="52" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Q11" s="52" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="R11" s="59"/>
       <c r="JC11" s="32"/>
@@ -8212,19 +8212,19 @@
         <v>3</v>
       </c>
       <c r="B12" s="53" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C12" s="54" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D12" s="73" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E12" s="56" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F12" s="56" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G12" s="141">
         <v>3</v>
@@ -8233,34 +8233,34 @@
         <v>1</v>
       </c>
       <c r="I12" s="139" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J12" s="137" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K12" s="35"/>
       <c r="L12" s="53" t="s">
+        <v>283</v>
+      </c>
+      <c r="M12" s="175" t="s">
+        <v>216</v>
+      </c>
+      <c r="N12" s="175" t="s">
         <v>284</v>
       </c>
-      <c r="M12" s="175" t="s">
+      <c r="O12" s="52" t="s">
         <v>217</v>
       </c>
-      <c r="N12" s="175" t="s">
-        <v>285</v>
-      </c>
-      <c r="O12" s="52" t="s">
-        <v>218</v>
-      </c>
       <c r="P12" s="52" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Q12" s="52" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="R12" s="59"/>
       <c r="JC12" s="142"/>
       <c r="JD12" s="143" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="JE12" s="129"/>
       <c r="JF12" s="129"/>
@@ -8273,19 +8273,19 @@
         <v>4</v>
       </c>
       <c r="B13" s="53" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C13" s="91" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D13" s="73" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E13" s="56" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F13" s="56" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G13" s="141">
         <v>1</v>
@@ -8294,36 +8294,36 @@
         <v>3</v>
       </c>
       <c r="I13" s="139" t="s">
+        <v>36</v>
+      </c>
+      <c r="J13" s="137" t="s">
         <v>37</v>
-      </c>
-      <c r="J13" s="137" t="s">
-        <v>38</v>
       </c>
       <c r="K13" s="35"/>
       <c r="L13" s="53" t="s">
+        <v>286</v>
+      </c>
+      <c r="M13" s="175" t="s">
         <v>287</v>
       </c>
-      <c r="M13" s="175" t="s">
+      <c r="N13" s="175" t="s">
+        <v>218</v>
+      </c>
+      <c r="O13" s="52" t="s">
+        <v>219</v>
+      </c>
+      <c r="P13" s="52" t="s">
         <v>288</v>
       </c>
-      <c r="N13" s="175" t="s">
-        <v>219</v>
-      </c>
-      <c r="O13" s="52" t="s">
-        <v>220</v>
-      </c>
-      <c r="P13" s="52" t="s">
-        <v>289</v>
-      </c>
       <c r="Q13" s="52" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="R13" s="59"/>
       <c r="JC13" s="50" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="JD13" s="51" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="JE13" s="129"/>
       <c r="JF13" s="130"/>
@@ -8356,11 +8356,11 @@
         <v>1</v>
       </c>
       <c r="JD14" s="47" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="JE14" s="129"/>
       <c r="JF14" s="130" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="JG14" s="130"/>
       <c r="JH14" s="128"/>
@@ -8391,11 +8391,11 @@
         <v>2</v>
       </c>
       <c r="JD15" s="48" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="JE15" s="130"/>
       <c r="JF15" s="130" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="JG15" s="130"/>
       <c r="JH15" s="127"/>
@@ -8424,11 +8424,11 @@
         <v>3</v>
       </c>
       <c r="JD16" s="47" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="JE16" s="130"/>
       <c r="JF16" s="131" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="JG16" s="129"/>
       <c r="JH16" s="127"/>
@@ -8457,11 +8457,11 @@
         <v>4</v>
       </c>
       <c r="JD17" s="47" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="JE17" s="130"/>
       <c r="JF17" s="131" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="JG17" s="129"/>
       <c r="JH17" s="127"/>
@@ -8490,11 +8490,11 @@
         <v>5</v>
       </c>
       <c r="JD18" s="47" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="JE18" s="129"/>
       <c r="JF18" s="131" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="JG18" s="129"/>
       <c r="JH18" s="128"/>
@@ -8520,14 +8520,14 @@
       <c r="Q19" s="52"/>
       <c r="R19" s="59"/>
       <c r="JC19" s="50" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="JD19" s="44" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="JE19" s="129"/>
       <c r="JF19" s="130" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="JG19" s="130"/>
       <c r="JH19" s="128"/>
@@ -8556,11 +8556,11 @@
         <v>1</v>
       </c>
       <c r="JD20" s="46" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="JE20" s="129"/>
       <c r="JF20" s="130" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="JG20" s="130"/>
       <c r="JH20" s="128"/>
@@ -8590,7 +8590,7 @@
         <v>2</v>
       </c>
       <c r="JD21" s="49" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="JE21" s="130"/>
       <c r="JF21" s="130"/>
@@ -8618,16 +8618,16 @@
       <c r="Q22" s="52"/>
       <c r="R22" s="59"/>
       <c r="AP22" s="37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AQ22" s="37" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="JC22" s="43">
         <v>3</v>
       </c>
       <c r="JD22" s="48" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="JE22" s="130"/>
       <c r="JF22" s="130"/>
@@ -8649,16 +8649,16 @@
       <c r="K23" s="31"/>
       <c r="L23" s="33"/>
       <c r="AP23" s="35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AQ23" s="35" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="JC23" s="43">
         <v>4</v>
       </c>
       <c r="JD23" s="47" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="JE23" s="130"/>
       <c r="JF23" s="129"/>
@@ -8683,7 +8683,7 @@
         <v>5</v>
       </c>
       <c r="JD24" s="46" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="JE24" s="34"/>
       <c r="JF24" s="32"/>
@@ -8697,10 +8697,10 @@
       <c r="K25" s="31"/>
       <c r="L25" s="33"/>
       <c r="JC25" s="72" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="JD25" s="45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="JE25" s="34"/>
       <c r="JF25" s="32"/>
@@ -8717,7 +8717,7 @@
         <v>1</v>
       </c>
       <c r="JD26" s="43" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="JE26" s="32"/>
       <c r="JF26" s="32"/>
@@ -8734,7 +8734,7 @@
         <v>2</v>
       </c>
       <c r="JD27" s="43" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="JE27" s="32"/>
       <c r="JF27" s="32"/>
@@ -8751,7 +8751,7 @@
         <v>3</v>
       </c>
       <c r="JD28" s="43" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="JE28" s="32"/>
       <c r="JF28" s="32"/>
@@ -8768,7 +8768,7 @@
         <v>4</v>
       </c>
       <c r="JD29" s="43" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="JE29" s="32"/>
       <c r="JF29" s="32"/>
@@ -8783,16 +8783,16 @@
       <c r="L30" s="33"/>
       <c r="JC30" s="44"/>
       <c r="JD30" s="44" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="JE30" s="121" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="JF30" s="121" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="JG30" s="121" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="JH30" s="32"/>
       <c r="JI30" s="32"/>
@@ -8804,16 +8804,16 @@
       <c r="L31" s="33"/>
       <c r="JC31" s="108"/>
       <c r="JD31" s="111" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="JE31" s="123" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="JF31" s="124" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="JG31" s="124" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="JH31" s="32"/>
       <c r="JI31" s="32"/>
@@ -8825,16 +8825,16 @@
       <c r="L32" s="33"/>
       <c r="JC32" s="109"/>
       <c r="JD32" s="111" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="JE32" s="123" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="JF32" s="123" t="s">
+        <v>127</v>
+      </c>
+      <c r="JG32" s="124" t="s">
         <v>128</v>
-      </c>
-      <c r="JG32" s="124" t="s">
-        <v>129</v>
       </c>
       <c r="JH32" s="32"/>
       <c r="JI32" s="32"/>
@@ -8846,16 +8846,16 @@
       <c r="L33" s="33"/>
       <c r="JC33" s="110"/>
       <c r="JD33" s="111" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="JE33" s="123" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="JF33" s="124" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="JG33" s="124" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="JH33" s="32"/>
       <c r="JI33" s="32"/>
@@ -8866,10 +8866,10 @@
       <c r="K34" s="33"/>
       <c r="L34" s="41"/>
       <c r="JC34" s="45" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="JD34" s="45" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="JE34" s="32"/>
       <c r="JF34" s="32"/>
@@ -8886,7 +8886,7 @@
         <v>1</v>
       </c>
       <c r="JD35" s="43" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="JE35" s="32"/>
       <c r="JF35" s="32"/>
@@ -8903,7 +8903,7 @@
         <v>2</v>
       </c>
       <c r="JD36" s="43" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="JE36" s="32"/>
       <c r="JF36" s="32"/>
@@ -8920,7 +8920,7 @@
         <v>3</v>
       </c>
       <c r="JD37" s="43" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="JE37" s="32"/>
       <c r="JF37" s="32"/>
@@ -8937,7 +8937,7 @@
         <v>4</v>
       </c>
       <c r="JD38" s="43" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="JE38" s="32"/>
       <c r="JF38" s="32"/>
@@ -9143,10 +9143,10 @@
     <row r="64" spans="1:17" s="31" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A64" s="32"/>
       <c r="B64" s="122" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C64" s="122" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D64" s="32"/>
       <c r="E64" s="32"/>
@@ -9163,10 +9163,10 @@
     <row r="65" spans="1:17" s="31" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A65" s="32"/>
       <c r="B65" s="122" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C65" s="122" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D65" s="32"/>
       <c r="E65" s="32"/>
@@ -9183,10 +9183,10 @@
     <row r="66" spans="1:17" s="31" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A66" s="32"/>
       <c r="B66" s="122" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C66" s="122" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D66" s="32"/>
       <c r="E66" s="32"/>
@@ -10141,22 +10141,22 @@
     <row r="1" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="92" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="157" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="157" t="s">
         <v>83</v>
       </c>
-      <c r="B3" s="157" t="s">
-        <v>84</v>
-      </c>
     </row>
     <row r="4" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="192" t="s">
-        <v>137</v>
-      </c>
-      <c r="B4" s="193"/>
+      <c r="A4" s="193" t="s">
+        <v>136</v>
+      </c>
+      <c r="B4" s="194"/>
       <c r="D4" s="93"/>
       <c r="E4" s="100"/>
       <c r="F4" s="100"/>
@@ -10165,39 +10165,39 @@
     </row>
     <row r="5" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="95" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B5" s="94" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D5" s="93"/>
       <c r="E5" s="100"/>
       <c r="F5" s="100"/>
       <c r="G5" s="100" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H5" s="100"/>
     </row>
     <row r="6" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="97" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B6" s="94" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D6" s="93"/>
       <c r="E6" s="100"/>
       <c r="F6" s="100"/>
       <c r="G6" s="100" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H6" s="100"/>
     </row>
     <row r="7" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="194" t="s">
-        <v>245</v>
-      </c>
-      <c r="B7" s="195"/>
+      <c r="A7" s="195" t="s">
+        <v>244</v>
+      </c>
+      <c r="B7" s="196"/>
       <c r="E7" s="100"/>
       <c r="F7" s="100"/>
       <c r="G7" s="100"/>
@@ -10205,25 +10205,25 @@
     </row>
     <row r="8" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="95" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B8" s="94" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E8" s="100" t="s">
+        <v>89</v>
+      </c>
+      <c r="F8" s="100" t="s">
         <v>90</v>
-      </c>
-      <c r="F8" s="100" t="s">
-        <v>91</v>
       </c>
       <c r="G8" s="100"/>
       <c r="H8" s="100"/>
     </row>
     <row r="9" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="190" t="s">
-        <v>139</v>
-      </c>
-      <c r="B9" s="191"/>
+      <c r="A9" s="191" t="s">
+        <v>138</v>
+      </c>
+      <c r="B9" s="192"/>
       <c r="C9" s="100"/>
       <c r="D9" s="100"/>
       <c r="E9" s="100"/>
@@ -10233,10 +10233,10 @@
     </row>
     <row r="10" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="97" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B10" s="94" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C10" s="100"/>
       <c r="D10" s="100"/>
@@ -10246,10 +10246,10 @@
       <c r="H10" s="100"/>
     </row>
     <row r="11" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="190" t="s">
-        <v>140</v>
-      </c>
-      <c r="B11" s="191"/>
+      <c r="A11" s="191" t="s">
+        <v>139</v>
+      </c>
+      <c r="B11" s="192"/>
       <c r="C11" s="100"/>
       <c r="D11" s="100"/>
       <c r="E11" s="100"/>
@@ -10259,10 +10259,10 @@
     </row>
     <row r="12" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="97" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B12" s="94" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C12" s="100"/>
       <c r="D12" s="100"/>
@@ -10273,10 +10273,10 @@
     </row>
     <row r="13" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="99" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B13" s="94" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C13" s="100"/>
       <c r="D13" s="100"/>
@@ -10287,27 +10287,27 @@
     </row>
     <row r="14" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="99" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B14" s="94" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C14" s="100"/>
       <c r="D14" s="100" t="s">
+        <v>91</v>
+      </c>
+      <c r="E14" s="100" t="s">
         <v>92</v>
-      </c>
-      <c r="E14" s="100" t="s">
-        <v>93</v>
       </c>
       <c r="F14" s="100"/>
       <c r="G14" s="100"/>
       <c r="H14" s="100"/>
     </row>
     <row r="15" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="190" t="s">
-        <v>144</v>
-      </c>
-      <c r="B15" s="191"/>
+      <c r="A15" s="191" t="s">
+        <v>143</v>
+      </c>
+      <c r="B15" s="192"/>
       <c r="C15" s="100"/>
       <c r="D15" s="100"/>
       <c r="E15" s="100"/>
@@ -10317,10 +10317,10 @@
     </row>
     <row r="16" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="97" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B16" s="94" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C16" s="100"/>
       <c r="D16" s="100"/>
@@ -10330,8 +10330,8 @@
       <c r="H16" s="100"/>
     </row>
     <row r="17" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="190"/>
-      <c r="B17" s="191"/>
+      <c r="A17" s="191"/>
+      <c r="B17" s="192"/>
       <c r="C17" s="100"/>
       <c r="D17" s="100"/>
       <c r="E17" s="100"/>
@@ -10350,8 +10350,8 @@
       <c r="H18" s="100"/>
     </row>
     <row r="19" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="190"/>
-      <c r="B19" s="191"/>
+      <c r="A19" s="191"/>
+      <c r="B19" s="192"/>
       <c r="C19" s="100"/>
       <c r="D19" s="100"/>
       <c r="E19" s="100"/>
@@ -10384,18 +10384,18 @@
       <c r="B22" s="98"/>
       <c r="C22" s="100"/>
       <c r="D22" s="100" t="s">
+        <v>93</v>
+      </c>
+      <c r="E22" s="100" t="s">
         <v>94</v>
-      </c>
-      <c r="E22" s="100" t="s">
-        <v>95</v>
       </c>
       <c r="F22" s="100"/>
       <c r="G22" s="100"/>
       <c r="H22" s="100"/>
     </row>
     <row r="23" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="190"/>
-      <c r="B23" s="191"/>
+      <c r="A23" s="191"/>
+      <c r="B23" s="192"/>
       <c r="C23" s="100"/>
       <c r="D23" s="100"/>
       <c r="E23" s="100"/>
@@ -10422,8 +10422,8 @@
       <c r="G25" s="100"/>
     </row>
     <row r="26" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="190"/>
-      <c r="B26" s="191"/>
+      <c r="A26" s="191"/>
+      <c r="B26" s="192"/>
       <c r="C26" s="100"/>
       <c r="D26" s="100"/>
       <c r="E26" s="100"/>
@@ -10435,17 +10435,17 @@
       <c r="B27" s="98"/>
       <c r="C27" s="100"/>
       <c r="D27" s="100" t="s">
+        <v>95</v>
+      </c>
+      <c r="E27" s="100" t="s">
         <v>96</v>
-      </c>
-      <c r="E27" s="100" t="s">
-        <v>97</v>
       </c>
       <c r="F27" s="100"/>
       <c r="G27" s="100"/>
     </row>
     <row r="28" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="190"/>
-      <c r="B28" s="191"/>
+      <c r="A28" s="191"/>
+      <c r="B28" s="192"/>
       <c r="C28" s="100"/>
       <c r="D28" s="100"/>
       <c r="E28" s="100"/>
@@ -10462,8 +10462,8 @@
       <c r="G29" s="100"/>
     </row>
     <row r="30" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="190"/>
-      <c r="B30" s="191"/>
+      <c r="A30" s="191"/>
+      <c r="B30" s="192"/>
       <c r="C30" s="100"/>
       <c r="D30" s="100"/>
       <c r="E30" s="100"/>
@@ -10475,10 +10475,10 @@
       <c r="B31" s="94"/>
       <c r="C31" s="100"/>
       <c r="D31" s="100" t="s">
+        <v>95</v>
+      </c>
+      <c r="E31" s="100" t="s">
         <v>96</v>
-      </c>
-      <c r="E31" s="100" t="s">
-        <v>97</v>
       </c>
       <c r="F31" s="100"/>
       <c r="G31" s="100"/>
@@ -10493,8 +10493,8 @@
       <c r="G32" s="100"/>
     </row>
     <row r="33" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="190"/>
-      <c r="B33" s="191"/>
+      <c r="A33" s="191"/>
+      <c r="B33" s="192"/>
       <c r="C33" s="100"/>
       <c r="D33" s="100"/>
       <c r="E33" s="100"/>
@@ -10506,10 +10506,10 @@
       <c r="B34" s="94"/>
       <c r="C34" s="100"/>
       <c r="D34" s="100" t="s">
+        <v>95</v>
+      </c>
+      <c r="E34" s="100" t="s">
         <v>96</v>
-      </c>
-      <c r="E34" s="100" t="s">
-        <v>97</v>
       </c>
       <c r="F34" s="100"/>
       <c r="G34" s="100"/>
@@ -10606,92 +10606,92 @@
     </row>
     <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="157" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B3" s="158" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C3" s="113"/>
     </row>
     <row r="4" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="125" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B4" s="114" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C4" s="113"/>
       <c r="D4" s="100"/>
       <c r="E4" s="100"/>
       <c r="F4" s="100"/>
       <c r="G4" s="100" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H4" s="100"/>
     </row>
     <row r="5" spans="1:10" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="126" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B5" s="114" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C5" s="113"/>
       <c r="D5" s="100"/>
       <c r="E5" s="100"/>
       <c r="F5" s="100"/>
       <c r="G5" s="100" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H5" s="100"/>
     </row>
     <row r="6" spans="1:10" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="126" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B6" s="114" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C6" s="113"/>
       <c r="D6" s="100"/>
       <c r="E6" s="100"/>
       <c r="F6" s="100"/>
       <c r="G6" s="100" t="s">
+        <v>87</v>
+      </c>
+      <c r="H6" s="100" t="s">
         <v>88</v>
-      </c>
-      <c r="H6" s="100" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="157" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="157" t="s">
         <v>99</v>
       </c>
-      <c r="B7" s="157" t="s">
-        <v>100</v>
-      </c>
       <c r="C7" s="159" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A8" s="125" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B8" s="101" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C8" s="94" t="s">
+        <v>101</v>
+      </c>
+      <c r="E8" s="100" t="s">
+        <v>89</v>
+      </c>
+      <c r="F8" s="100" t="s">
+        <v>101</v>
+      </c>
+      <c r="G8" s="100" t="s">
         <v>102</v>
-      </c>
-      <c r="E8" s="100" t="s">
-        <v>90</v>
-      </c>
-      <c r="F8" s="100" t="s">
-        <v>102</v>
-      </c>
-      <c r="G8" s="100" t="s">
-        <v>103</v>
       </c>
       <c r="H8" s="100"/>
       <c r="I8" s="100"/>
@@ -10699,13 +10699,13 @@
     </row>
     <row r="9" spans="1:10" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="126" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B9" s="102" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C9" s="94" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E9" s="100"/>
       <c r="F9" s="100"/>
@@ -10716,13 +10716,13 @@
     </row>
     <row r="10" spans="1:10" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="176" t="s">
+        <v>297</v>
+      </c>
+      <c r="B10" s="103" t="s">
         <v>298</v>
       </c>
-      <c r="B10" s="103" t="s">
-        <v>299</v>
-      </c>
       <c r="C10" s="94" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E10" s="100"/>
       <c r="F10" s="100"/>
@@ -10731,13 +10731,13 @@
     </row>
     <row r="11" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="126" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B11" s="102" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C11" s="94" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E11" s="100"/>
       <c r="F11" s="100"/>
@@ -10746,13 +10746,13 @@
     </row>
     <row r="12" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="126" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B12" s="102" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C12" s="94" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D12" s="100"/>
       <c r="E12" s="100"/>
@@ -10762,13 +10762,13 @@
     </row>
     <row r="13" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="126" t="s">
+        <v>235</v>
+      </c>
+      <c r="B13" s="104" t="s">
         <v>236</v>
       </c>
-      <c r="B13" s="104" t="s">
-        <v>237</v>
-      </c>
       <c r="C13" s="94" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D13" s="100"/>
       <c r="E13" s="100"/>
@@ -10778,13 +10778,13 @@
     </row>
     <row r="14" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="126" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B14" s="104" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C14" s="94" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D14" s="100"/>
       <c r="E14" s="100"/>
@@ -10794,13 +10794,13 @@
     </row>
     <row r="15" spans="1:10" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="126" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B15" s="101" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C15" s="94" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D15" s="100"/>
       <c r="E15" s="100"/>
@@ -10810,13 +10810,13 @@
     </row>
     <row r="16" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="126" t="s">
+        <v>239</v>
+      </c>
+      <c r="B16" s="102" t="s">
         <v>240</v>
       </c>
-      <c r="B16" s="102" t="s">
-        <v>241</v>
-      </c>
       <c r="C16" s="94" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D16" s="100"/>
       <c r="E16" s="100"/>
@@ -11754,7 +11754,7 @@
     <row r="2" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="148"/>
       <c r="B2" s="149" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C2" s="148"/>
       <c r="D2" s="148"/>
@@ -11765,51 +11765,51 @@
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>105</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>106</v>
       </c>
       <c r="G3" s="116"/>
       <c r="H3" s="116" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I3" s="116" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="10"/>
       <c r="B4" s="67" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G4" s="116"/>
       <c r="H4" s="116" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I4" s="116" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="10"/>
       <c r="B5" s="67" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G5" s="116"/>
       <c r="H5" s="116"/>
@@ -11817,109 +11817,109 @@
     </row>
     <row r="6" spans="1:9" s="10" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B6" s="62" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G6" s="117"/>
       <c r="H6" s="117"/>
       <c r="I6" s="116" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="10" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B7" s="62" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G7" s="117"/>
       <c r="H7" s="117"/>
       <c r="I7" s="116" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="10" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B8" s="62" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G8" s="117"/>
       <c r="H8" s="117"/>
       <c r="I8" s="118" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B9" s="62" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G9" s="117"/>
       <c r="H9" s="117"/>
       <c r="I9" s="118" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="10" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B10" s="62" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G10" s="117"/>
       <c r="H10" s="117"/>
       <c r="I10" s="118" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="10" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B11" s="62" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G11" s="117"/>
       <c r="H11" s="117"/>
       <c r="I11" s="118" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B12" s="62" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G12" s="117"/>
       <c r="H12" s="117"/>
@@ -11927,13 +11927,13 @@
     </row>
     <row r="13" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B13" s="62" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G13" s="116"/>
       <c r="H13" s="116"/>
@@ -12757,7 +12757,7 @@
     <row r="2" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="148"/>
       <c r="B2" s="149" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C2" s="148"/>
       <c r="D2" s="148"/>
@@ -12767,82 +12767,82 @@
     </row>
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
-      <c r="B3" s="197" t="s">
-        <v>115</v>
-      </c>
-      <c r="C3" s="197"/>
-      <c r="D3" s="197"/>
+      <c r="B3" s="198" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" s="198"/>
+      <c r="D3" s="198"/>
       <c r="G3" s="116"/>
       <c r="H3" s="116" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I3" s="116" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10"/>
-      <c r="B4" s="196" t="s">
-        <v>306</v>
-      </c>
-      <c r="C4" s="196"/>
-      <c r="D4" s="196"/>
+      <c r="B4" s="197" t="s">
+        <v>305</v>
+      </c>
+      <c r="C4" s="197"/>
+      <c r="D4" s="197"/>
       <c r="G4" s="116"/>
       <c r="H4" s="116" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I4" s="116" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="196" t="s">
-        <v>305</v>
-      </c>
-      <c r="C5" s="196"/>
-      <c r="D5" s="196"/>
+      <c r="B5" s="197" t="s">
+        <v>304</v>
+      </c>
+      <c r="C5" s="197"/>
+      <c r="D5" s="197"/>
       <c r="G5" s="117"/>
       <c r="H5" s="117"/>
       <c r="I5" s="116" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="196" t="s">
-        <v>117</v>
-      </c>
-      <c r="C6" s="196"/>
-      <c r="D6" s="196"/>
+      <c r="B6" s="197" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6" s="197"/>
+      <c r="D6" s="197"/>
       <c r="G6" s="117"/>
       <c r="H6" s="117"/>
       <c r="I6" s="118"/>
     </row>
     <row r="7" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="196" t="s">
-        <v>118</v>
-      </c>
-      <c r="C7" s="196"/>
-      <c r="D7" s="196"/>
+      <c r="B7" s="197" t="s">
+        <v>117</v>
+      </c>
+      <c r="C7" s="197"/>
+      <c r="D7" s="197"/>
       <c r="G7" s="117"/>
       <c r="H7" s="117"/>
       <c r="I7" s="118"/>
     </row>
     <row r="8" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="196" t="s">
-        <v>119</v>
-      </c>
-      <c r="C8" s="196"/>
-      <c r="D8" s="196"/>
+      <c r="B8" s="197" t="s">
+        <v>118</v>
+      </c>
+      <c r="C8" s="197"/>
+      <c r="D8" s="197"/>
       <c r="G8" s="117"/>
       <c r="H8" s="117"/>
       <c r="I8" s="118"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B9" s="196" t="s">
-        <v>120</v>
-      </c>
-      <c r="C9" s="196"/>
-      <c r="D9" s="196"/>
+      <c r="B9" s="197" t="s">
+        <v>119</v>
+      </c>
+      <c r="C9" s="197"/>
+      <c r="D9" s="197"/>
       <c r="G9" s="117"/>
       <c r="H9" s="117"/>
       <c r="I9" s="118"/>
@@ -12860,7 +12860,7 @@
     <row r="12" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="148"/>
       <c r="B12" s="149" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C12" s="148"/>
       <c r="D12" s="148"/>
@@ -12870,88 +12870,95 @@
     </row>
     <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
-      <c r="B13" s="197" t="s">
-        <v>115</v>
-      </c>
-      <c r="C13" s="197"/>
-      <c r="D13" s="197"/>
+      <c r="B13" s="198" t="s">
+        <v>114</v>
+      </c>
+      <c r="C13" s="198"/>
+      <c r="D13" s="198"/>
       <c r="G13" s="116"/>
       <c r="H13" s="116" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I13" s="116" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="10"/>
-      <c r="B14" s="196" t="s">
-        <v>182</v>
-      </c>
-      <c r="C14" s="196"/>
-      <c r="D14" s="196"/>
+      <c r="B14" s="197" t="s">
+        <v>181</v>
+      </c>
+      <c r="C14" s="197"/>
+      <c r="D14" s="197"/>
       <c r="G14" s="116"/>
       <c r="H14" s="116" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I14" s="116" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="196" t="s">
-        <v>183</v>
-      </c>
-      <c r="C15" s="196"/>
-      <c r="D15" s="196"/>
+      <c r="B15" s="197" t="s">
+        <v>182</v>
+      </c>
+      <c r="C15" s="197"/>
+      <c r="D15" s="197"/>
       <c r="G15" s="117"/>
       <c r="H15" s="117"/>
       <c r="I15" s="116" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="196" t="s">
-        <v>227</v>
-      </c>
-      <c r="C16" s="196"/>
-      <c r="D16" s="196"/>
+      <c r="B16" s="197" t="s">
+        <v>226</v>
+      </c>
+      <c r="C16" s="197"/>
+      <c r="D16" s="197"/>
       <c r="G16" s="117"/>
       <c r="H16" s="117"/>
       <c r="I16" s="118"/>
     </row>
     <row r="17" spans="2:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="196" t="s">
-        <v>228</v>
-      </c>
-      <c r="C17" s="196"/>
-      <c r="D17" s="196"/>
+      <c r="B17" s="197" t="s">
+        <v>227</v>
+      </c>
+      <c r="C17" s="197"/>
+      <c r="D17" s="197"/>
       <c r="G17" s="117"/>
       <c r="H17" s="117"/>
       <c r="I17" s="118"/>
     </row>
     <row r="18" spans="2:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="196" t="s">
-        <v>119</v>
-      </c>
-      <c r="C18" s="196"/>
-      <c r="D18" s="196"/>
+      <c r="B18" s="197" t="s">
+        <v>118</v>
+      </c>
+      <c r="C18" s="197"/>
+      <c r="D18" s="197"/>
       <c r="G18" s="117"/>
       <c r="H18" s="117"/>
       <c r="I18" s="118"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B19" s="196" t="s">
-        <v>120</v>
-      </c>
-      <c r="C19" s="196"/>
-      <c r="D19" s="196"/>
+      <c r="B19" s="197" t="s">
+        <v>119</v>
+      </c>
+      <c r="C19" s="197"/>
+      <c r="D19" s="197"/>
       <c r="G19" s="117"/>
       <c r="H19" s="117"/>
       <c r="I19" s="118"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="B3:D3"/>
@@ -12959,13 +12966,6 @@
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B18:D18"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="IS65533:IS65542 SO65533:SO65542 ACK65533:ACK65542 AMG65533:AMG65542 AWC65533:AWC65542 BFY65533:BFY65542 BPU65533:BPU65542 BZQ65533:BZQ65542 CJM65533:CJM65542 CTI65533:CTI65542 DDE65533:DDE65542 DNA65533:DNA65542 DWW65533:DWW65542 EGS65533:EGS65542 EQO65533:EQO65542 FAK65533:FAK65542 FKG65533:FKG65542 FUC65533:FUC65542 GDY65533:GDY65542 GNU65533:GNU65542 GXQ65533:GXQ65542 HHM65533:HHM65542 HRI65533:HRI65542 IBE65533:IBE65542 ILA65533:ILA65542 IUW65533:IUW65542 JES65533:JES65542 JOO65533:JOO65542 JYK65533:JYK65542 KIG65533:KIG65542 KSC65533:KSC65542 LBY65533:LBY65542 LLU65533:LLU65542 LVQ65533:LVQ65542 MFM65533:MFM65542 MPI65533:MPI65542 MZE65533:MZE65542 NJA65533:NJA65542 NSW65533:NSW65542 OCS65533:OCS65542 OMO65533:OMO65542 OWK65533:OWK65542 PGG65533:PGG65542 PQC65533:PQC65542 PZY65533:PZY65542 QJU65533:QJU65542 QTQ65533:QTQ65542 RDM65533:RDM65542 RNI65533:RNI65542 RXE65533:RXE65542 SHA65533:SHA65542 SQW65533:SQW65542 TAS65533:TAS65542 TKO65533:TKO65542 TUK65533:TUK65542 UEG65533:UEG65542 UOC65533:UOC65542 UXY65533:UXY65542 VHU65533:VHU65542 VRQ65533:VRQ65542 WBM65533:WBM65542 WLI65533:WLI65542 WVE65533:WVE65542 IS131069:IS131078 SO131069:SO131078 ACK131069:ACK131078 AMG131069:AMG131078 AWC131069:AWC131078 BFY131069:BFY131078 BPU131069:BPU131078 BZQ131069:BZQ131078 CJM131069:CJM131078 CTI131069:CTI131078 DDE131069:DDE131078 DNA131069:DNA131078 DWW131069:DWW131078 EGS131069:EGS131078 EQO131069:EQO131078 FAK131069:FAK131078 FKG131069:FKG131078 FUC131069:FUC131078 GDY131069:GDY131078 GNU131069:GNU131078 GXQ131069:GXQ131078 HHM131069:HHM131078 HRI131069:HRI131078 IBE131069:IBE131078 ILA131069:ILA131078 IUW131069:IUW131078 JES131069:JES131078 JOO131069:JOO131078 JYK131069:JYK131078 KIG131069:KIG131078 KSC131069:KSC131078 LBY131069:LBY131078 LLU131069:LLU131078 LVQ131069:LVQ131078 MFM131069:MFM131078 MPI131069:MPI131078 MZE131069:MZE131078 NJA131069:NJA131078 NSW131069:NSW131078 OCS131069:OCS131078 OMO131069:OMO131078 OWK131069:OWK131078 PGG131069:PGG131078 PQC131069:PQC131078 PZY131069:PZY131078 QJU131069:QJU131078 QTQ131069:QTQ131078 RDM131069:RDM131078 RNI131069:RNI131078 RXE131069:RXE131078 SHA131069:SHA131078 SQW131069:SQW131078 TAS131069:TAS131078 TKO131069:TKO131078 TUK131069:TUK131078 UEG131069:UEG131078 UOC131069:UOC131078 UXY131069:UXY131078 VHU131069:VHU131078 VRQ131069:VRQ131078 WBM131069:WBM131078 WLI131069:WLI131078 WVE131069:WVE131078 IS196605:IS196614 SO196605:SO196614 ACK196605:ACK196614 AMG196605:AMG196614 AWC196605:AWC196614 BFY196605:BFY196614 BPU196605:BPU196614 BZQ196605:BZQ196614 CJM196605:CJM196614 CTI196605:CTI196614 DDE196605:DDE196614 DNA196605:DNA196614 DWW196605:DWW196614 EGS196605:EGS196614 EQO196605:EQO196614 FAK196605:FAK196614 FKG196605:FKG196614 FUC196605:FUC196614 GDY196605:GDY196614 GNU196605:GNU196614 GXQ196605:GXQ196614 HHM196605:HHM196614 HRI196605:HRI196614 IBE196605:IBE196614 ILA196605:ILA196614 IUW196605:IUW196614 JES196605:JES196614 JOO196605:JOO196614 JYK196605:JYK196614 KIG196605:KIG196614 KSC196605:KSC196614 LBY196605:LBY196614 LLU196605:LLU196614 LVQ196605:LVQ196614 MFM196605:MFM196614 MPI196605:MPI196614 MZE196605:MZE196614 NJA196605:NJA196614 NSW196605:NSW196614 OCS196605:OCS196614 OMO196605:OMO196614 OWK196605:OWK196614 PGG196605:PGG196614 PQC196605:PQC196614 PZY196605:PZY196614 QJU196605:QJU196614 QTQ196605:QTQ196614 RDM196605:RDM196614 RNI196605:RNI196614 RXE196605:RXE196614 SHA196605:SHA196614 SQW196605:SQW196614 TAS196605:TAS196614 TKO196605:TKO196614 TUK196605:TUK196614 UEG196605:UEG196614 UOC196605:UOC196614 UXY196605:UXY196614 VHU196605:VHU196614 VRQ196605:VRQ196614 WBM196605:WBM196614 WLI196605:WLI196614 WVE196605:WVE196614 IS262141:IS262150 SO262141:SO262150 ACK262141:ACK262150 AMG262141:AMG262150 AWC262141:AWC262150 BFY262141:BFY262150 BPU262141:BPU262150 BZQ262141:BZQ262150 CJM262141:CJM262150 CTI262141:CTI262150 DDE262141:DDE262150 DNA262141:DNA262150 DWW262141:DWW262150 EGS262141:EGS262150 EQO262141:EQO262150 FAK262141:FAK262150 FKG262141:FKG262150 FUC262141:FUC262150 GDY262141:GDY262150 GNU262141:GNU262150 GXQ262141:GXQ262150 HHM262141:HHM262150 HRI262141:HRI262150 IBE262141:IBE262150 ILA262141:ILA262150 IUW262141:IUW262150 JES262141:JES262150 JOO262141:JOO262150 JYK262141:JYK262150 KIG262141:KIG262150 KSC262141:KSC262150 LBY262141:LBY262150 LLU262141:LLU262150 LVQ262141:LVQ262150 MFM262141:MFM262150 MPI262141:MPI262150 MZE262141:MZE262150 NJA262141:NJA262150 NSW262141:NSW262150 OCS262141:OCS262150 OMO262141:OMO262150 OWK262141:OWK262150 PGG262141:PGG262150 PQC262141:PQC262150 PZY262141:PZY262150 QJU262141:QJU262150 QTQ262141:QTQ262150 RDM262141:RDM262150 RNI262141:RNI262150 RXE262141:RXE262150 SHA262141:SHA262150 SQW262141:SQW262150 TAS262141:TAS262150 TKO262141:TKO262150 TUK262141:TUK262150 UEG262141:UEG262150 UOC262141:UOC262150 UXY262141:UXY262150 VHU262141:VHU262150 VRQ262141:VRQ262150 WBM262141:WBM262150 WLI262141:WLI262150 WVE262141:WVE262150 IS327677:IS327686 SO327677:SO327686 ACK327677:ACK327686 AMG327677:AMG327686 AWC327677:AWC327686 BFY327677:BFY327686 BPU327677:BPU327686 BZQ327677:BZQ327686 CJM327677:CJM327686 CTI327677:CTI327686 DDE327677:DDE327686 DNA327677:DNA327686 DWW327677:DWW327686 EGS327677:EGS327686 EQO327677:EQO327686 FAK327677:FAK327686 FKG327677:FKG327686 FUC327677:FUC327686 GDY327677:GDY327686 GNU327677:GNU327686 GXQ327677:GXQ327686 HHM327677:HHM327686 HRI327677:HRI327686 IBE327677:IBE327686 ILA327677:ILA327686 IUW327677:IUW327686 JES327677:JES327686 JOO327677:JOO327686 JYK327677:JYK327686 KIG327677:KIG327686 KSC327677:KSC327686 LBY327677:LBY327686 LLU327677:LLU327686 LVQ327677:LVQ327686 MFM327677:MFM327686 MPI327677:MPI327686 MZE327677:MZE327686 NJA327677:NJA327686 NSW327677:NSW327686 OCS327677:OCS327686 OMO327677:OMO327686 OWK327677:OWK327686 PGG327677:PGG327686 PQC327677:PQC327686 PZY327677:PZY327686 QJU327677:QJU327686 QTQ327677:QTQ327686 RDM327677:RDM327686 RNI327677:RNI327686 RXE327677:RXE327686 SHA327677:SHA327686 SQW327677:SQW327686 TAS327677:TAS327686 TKO327677:TKO327686 TUK327677:TUK327686 UEG327677:UEG327686 UOC327677:UOC327686 UXY327677:UXY327686 VHU327677:VHU327686 VRQ327677:VRQ327686 WBM327677:WBM327686 WLI327677:WLI327686 WVE327677:WVE327686 IS393213:IS393222 SO393213:SO393222 ACK393213:ACK393222 AMG393213:AMG393222 AWC393213:AWC393222 BFY393213:BFY393222 BPU393213:BPU393222 BZQ393213:BZQ393222 CJM393213:CJM393222 CTI393213:CTI393222 DDE393213:DDE393222 DNA393213:DNA393222 DWW393213:DWW393222 EGS393213:EGS393222 EQO393213:EQO393222 FAK393213:FAK393222 FKG393213:FKG393222 FUC393213:FUC393222 GDY393213:GDY393222 GNU393213:GNU393222 GXQ393213:GXQ393222 HHM393213:HHM393222 HRI393213:HRI393222 IBE393213:IBE393222 ILA393213:ILA393222 IUW393213:IUW393222 JES393213:JES393222 JOO393213:JOO393222 JYK393213:JYK393222 KIG393213:KIG393222 KSC393213:KSC393222 LBY393213:LBY393222 LLU393213:LLU393222 LVQ393213:LVQ393222 MFM393213:MFM393222 MPI393213:MPI393222 MZE393213:MZE393222 NJA393213:NJA393222 NSW393213:NSW393222 OCS393213:OCS393222 OMO393213:OMO393222 OWK393213:OWK393222 PGG393213:PGG393222 PQC393213:PQC393222 PZY393213:PZY393222 QJU393213:QJU393222 QTQ393213:QTQ393222 RDM393213:RDM393222 RNI393213:RNI393222 RXE393213:RXE393222 SHA393213:SHA393222 SQW393213:SQW393222 TAS393213:TAS393222 TKO393213:TKO393222 TUK393213:TUK393222 UEG393213:UEG393222 UOC393213:UOC393222 UXY393213:UXY393222 VHU393213:VHU393222 VRQ393213:VRQ393222 WBM393213:WBM393222 WLI393213:WLI393222 WVE393213:WVE393222 IS458749:IS458758 SO458749:SO458758 ACK458749:ACK458758 AMG458749:AMG458758 AWC458749:AWC458758 BFY458749:BFY458758 BPU458749:BPU458758 BZQ458749:BZQ458758 CJM458749:CJM458758 CTI458749:CTI458758 DDE458749:DDE458758 DNA458749:DNA458758 DWW458749:DWW458758 EGS458749:EGS458758 EQO458749:EQO458758 FAK458749:FAK458758 FKG458749:FKG458758 FUC458749:FUC458758 GDY458749:GDY458758 GNU458749:GNU458758 GXQ458749:GXQ458758 HHM458749:HHM458758 HRI458749:HRI458758 IBE458749:IBE458758 ILA458749:ILA458758 IUW458749:IUW458758 JES458749:JES458758 JOO458749:JOO458758 JYK458749:JYK458758 KIG458749:KIG458758 KSC458749:KSC458758 LBY458749:LBY458758 LLU458749:LLU458758 LVQ458749:LVQ458758 MFM458749:MFM458758 MPI458749:MPI458758 MZE458749:MZE458758 NJA458749:NJA458758 NSW458749:NSW458758 OCS458749:OCS458758 OMO458749:OMO458758 OWK458749:OWK458758 PGG458749:PGG458758 PQC458749:PQC458758 PZY458749:PZY458758 QJU458749:QJU458758 QTQ458749:QTQ458758 RDM458749:RDM458758 RNI458749:RNI458758 RXE458749:RXE458758 SHA458749:SHA458758 SQW458749:SQW458758 TAS458749:TAS458758 TKO458749:TKO458758 TUK458749:TUK458758 UEG458749:UEG458758 UOC458749:UOC458758 UXY458749:UXY458758 VHU458749:VHU458758 VRQ458749:VRQ458758 WBM458749:WBM458758 WLI458749:WLI458758 WVE458749:WVE458758 IS524285:IS524294 SO524285:SO524294 ACK524285:ACK524294 AMG524285:AMG524294 AWC524285:AWC524294 BFY524285:BFY524294 BPU524285:BPU524294 BZQ524285:BZQ524294 CJM524285:CJM524294 CTI524285:CTI524294 DDE524285:DDE524294 DNA524285:DNA524294 DWW524285:DWW524294 EGS524285:EGS524294 EQO524285:EQO524294 FAK524285:FAK524294 FKG524285:FKG524294 FUC524285:FUC524294 GDY524285:GDY524294 GNU524285:GNU524294 GXQ524285:GXQ524294 HHM524285:HHM524294 HRI524285:HRI524294 IBE524285:IBE524294 ILA524285:ILA524294 IUW524285:IUW524294 JES524285:JES524294 JOO524285:JOO524294 JYK524285:JYK524294 KIG524285:KIG524294 KSC524285:KSC524294 LBY524285:LBY524294 LLU524285:LLU524294 LVQ524285:LVQ524294 MFM524285:MFM524294 MPI524285:MPI524294 MZE524285:MZE524294 NJA524285:NJA524294 NSW524285:NSW524294 OCS524285:OCS524294 OMO524285:OMO524294 OWK524285:OWK524294 PGG524285:PGG524294 PQC524285:PQC524294 PZY524285:PZY524294 QJU524285:QJU524294 QTQ524285:QTQ524294 RDM524285:RDM524294 RNI524285:RNI524294 RXE524285:RXE524294 SHA524285:SHA524294 SQW524285:SQW524294 TAS524285:TAS524294 TKO524285:TKO524294 TUK524285:TUK524294 UEG524285:UEG524294 UOC524285:UOC524294 UXY524285:UXY524294 VHU524285:VHU524294 VRQ524285:VRQ524294 WBM524285:WBM524294 WLI524285:WLI524294 WVE524285:WVE524294 IS589821:IS589830 SO589821:SO589830 ACK589821:ACK589830 AMG589821:AMG589830 AWC589821:AWC589830 BFY589821:BFY589830 BPU589821:BPU589830 BZQ589821:BZQ589830 CJM589821:CJM589830 CTI589821:CTI589830 DDE589821:DDE589830 DNA589821:DNA589830 DWW589821:DWW589830 EGS589821:EGS589830 EQO589821:EQO589830 FAK589821:FAK589830 FKG589821:FKG589830 FUC589821:FUC589830 GDY589821:GDY589830 GNU589821:GNU589830 GXQ589821:GXQ589830 HHM589821:HHM589830 HRI589821:HRI589830 IBE589821:IBE589830 ILA589821:ILA589830 IUW589821:IUW589830 JES589821:JES589830 JOO589821:JOO589830 JYK589821:JYK589830 KIG589821:KIG589830 KSC589821:KSC589830 LBY589821:LBY589830 LLU589821:LLU589830 LVQ589821:LVQ589830 MFM589821:MFM589830 MPI589821:MPI589830 MZE589821:MZE589830 NJA589821:NJA589830 NSW589821:NSW589830 OCS589821:OCS589830 OMO589821:OMO589830 OWK589821:OWK589830 PGG589821:PGG589830 PQC589821:PQC589830 PZY589821:PZY589830 QJU589821:QJU589830 QTQ589821:QTQ589830 RDM589821:RDM589830 RNI589821:RNI589830 RXE589821:RXE589830 SHA589821:SHA589830 SQW589821:SQW589830 TAS589821:TAS589830 TKO589821:TKO589830 TUK589821:TUK589830 UEG589821:UEG589830 UOC589821:UOC589830 UXY589821:UXY589830 VHU589821:VHU589830 VRQ589821:VRQ589830 WBM589821:WBM589830 WLI589821:WLI589830 WVE589821:WVE589830 IS655357:IS655366 SO655357:SO655366 ACK655357:ACK655366 AMG655357:AMG655366 AWC655357:AWC655366 BFY655357:BFY655366 BPU655357:BPU655366 BZQ655357:BZQ655366 CJM655357:CJM655366 CTI655357:CTI655366 DDE655357:DDE655366 DNA655357:DNA655366 DWW655357:DWW655366 EGS655357:EGS655366 EQO655357:EQO655366 FAK655357:FAK655366 FKG655357:FKG655366 FUC655357:FUC655366 GDY655357:GDY655366 GNU655357:GNU655366 GXQ655357:GXQ655366 HHM655357:HHM655366 HRI655357:HRI655366 IBE655357:IBE655366 ILA655357:ILA655366 IUW655357:IUW655366 JES655357:JES655366 JOO655357:JOO655366 JYK655357:JYK655366 KIG655357:KIG655366 KSC655357:KSC655366 LBY655357:LBY655366 LLU655357:LLU655366 LVQ655357:LVQ655366 MFM655357:MFM655366 MPI655357:MPI655366 MZE655357:MZE655366 NJA655357:NJA655366 NSW655357:NSW655366 OCS655357:OCS655366 OMO655357:OMO655366 OWK655357:OWK655366 PGG655357:PGG655366 PQC655357:PQC655366 PZY655357:PZY655366 QJU655357:QJU655366 QTQ655357:QTQ655366 RDM655357:RDM655366 RNI655357:RNI655366 RXE655357:RXE655366 SHA655357:SHA655366 SQW655357:SQW655366 TAS655357:TAS655366 TKO655357:TKO655366 TUK655357:TUK655366 UEG655357:UEG655366 UOC655357:UOC655366 UXY655357:UXY655366 VHU655357:VHU655366 VRQ655357:VRQ655366 WBM655357:WBM655366 WLI655357:WLI655366 WVE655357:WVE655366 IS720893:IS720902 SO720893:SO720902 ACK720893:ACK720902 AMG720893:AMG720902 AWC720893:AWC720902 BFY720893:BFY720902 BPU720893:BPU720902 BZQ720893:BZQ720902 CJM720893:CJM720902 CTI720893:CTI720902 DDE720893:DDE720902 DNA720893:DNA720902 DWW720893:DWW720902 EGS720893:EGS720902 EQO720893:EQO720902 FAK720893:FAK720902 FKG720893:FKG720902 FUC720893:FUC720902 GDY720893:GDY720902 GNU720893:GNU720902 GXQ720893:GXQ720902 HHM720893:HHM720902 HRI720893:HRI720902 IBE720893:IBE720902 ILA720893:ILA720902 IUW720893:IUW720902 JES720893:JES720902 JOO720893:JOO720902 JYK720893:JYK720902 KIG720893:KIG720902 KSC720893:KSC720902 LBY720893:LBY720902 LLU720893:LLU720902 LVQ720893:LVQ720902 MFM720893:MFM720902 MPI720893:MPI720902 MZE720893:MZE720902 NJA720893:NJA720902 NSW720893:NSW720902 OCS720893:OCS720902 OMO720893:OMO720902 OWK720893:OWK720902 PGG720893:PGG720902 PQC720893:PQC720902 PZY720893:PZY720902 QJU720893:QJU720902 QTQ720893:QTQ720902 RDM720893:RDM720902 RNI720893:RNI720902 RXE720893:RXE720902 SHA720893:SHA720902 SQW720893:SQW720902 TAS720893:TAS720902 TKO720893:TKO720902 TUK720893:TUK720902 UEG720893:UEG720902 UOC720893:UOC720902 UXY720893:UXY720902 VHU720893:VHU720902 VRQ720893:VRQ720902 WBM720893:WBM720902 WLI720893:WLI720902 WVE720893:WVE720902 IS786429:IS786438 SO786429:SO786438 ACK786429:ACK786438 AMG786429:AMG786438 AWC786429:AWC786438 BFY786429:BFY786438 BPU786429:BPU786438 BZQ786429:BZQ786438 CJM786429:CJM786438 CTI786429:CTI786438 DDE786429:DDE786438 DNA786429:DNA786438 DWW786429:DWW786438 EGS786429:EGS786438 EQO786429:EQO786438 FAK786429:FAK786438 FKG786429:FKG786438 FUC786429:FUC786438 GDY786429:GDY786438 GNU786429:GNU786438 GXQ786429:GXQ786438 HHM786429:HHM786438 HRI786429:HRI786438 IBE786429:IBE786438 ILA786429:ILA786438 IUW786429:IUW786438 JES786429:JES786438 JOO786429:JOO786438 JYK786429:JYK786438 KIG786429:KIG786438 KSC786429:KSC786438 LBY786429:LBY786438 LLU786429:LLU786438 LVQ786429:LVQ786438 MFM786429:MFM786438 MPI786429:MPI786438 MZE786429:MZE786438 NJA786429:NJA786438 NSW786429:NSW786438 OCS786429:OCS786438 OMO786429:OMO786438 OWK786429:OWK786438 PGG786429:PGG786438 PQC786429:PQC786438 PZY786429:PZY786438 QJU786429:QJU786438 QTQ786429:QTQ786438 RDM786429:RDM786438 RNI786429:RNI786438 RXE786429:RXE786438 SHA786429:SHA786438 SQW786429:SQW786438 TAS786429:TAS786438 TKO786429:TKO786438 TUK786429:TUK786438 UEG786429:UEG786438 UOC786429:UOC786438 UXY786429:UXY786438 VHU786429:VHU786438 VRQ786429:VRQ786438 WBM786429:WBM786438 WLI786429:WLI786438 WVE786429:WVE786438 IS851965:IS851974 SO851965:SO851974 ACK851965:ACK851974 AMG851965:AMG851974 AWC851965:AWC851974 BFY851965:BFY851974 BPU851965:BPU851974 BZQ851965:BZQ851974 CJM851965:CJM851974 CTI851965:CTI851974 DDE851965:DDE851974 DNA851965:DNA851974 DWW851965:DWW851974 EGS851965:EGS851974 EQO851965:EQO851974 FAK851965:FAK851974 FKG851965:FKG851974 FUC851965:FUC851974 GDY851965:GDY851974 GNU851965:GNU851974 GXQ851965:GXQ851974 HHM851965:HHM851974 HRI851965:HRI851974 IBE851965:IBE851974 ILA851965:ILA851974 IUW851965:IUW851974 JES851965:JES851974 JOO851965:JOO851974 JYK851965:JYK851974 KIG851965:KIG851974 KSC851965:KSC851974 LBY851965:LBY851974 LLU851965:LLU851974 LVQ851965:LVQ851974 MFM851965:MFM851974 MPI851965:MPI851974 MZE851965:MZE851974 NJA851965:NJA851974 NSW851965:NSW851974 OCS851965:OCS851974 OMO851965:OMO851974 OWK851965:OWK851974 PGG851965:PGG851974 PQC851965:PQC851974 PZY851965:PZY851974 QJU851965:QJU851974 QTQ851965:QTQ851974 RDM851965:RDM851974 RNI851965:RNI851974 RXE851965:RXE851974 SHA851965:SHA851974 SQW851965:SQW851974 TAS851965:TAS851974 TKO851965:TKO851974 TUK851965:TUK851974 UEG851965:UEG851974 UOC851965:UOC851974 UXY851965:UXY851974 VHU851965:VHU851974 VRQ851965:VRQ851974 WBM851965:WBM851974 WLI851965:WLI851974 WVE851965:WVE851974 IS917501:IS917510 SO917501:SO917510 ACK917501:ACK917510 AMG917501:AMG917510 AWC917501:AWC917510 BFY917501:BFY917510 BPU917501:BPU917510 BZQ917501:BZQ917510 CJM917501:CJM917510 CTI917501:CTI917510 DDE917501:DDE917510 DNA917501:DNA917510 DWW917501:DWW917510 EGS917501:EGS917510 EQO917501:EQO917510 FAK917501:FAK917510 FKG917501:FKG917510 FUC917501:FUC917510 GDY917501:GDY917510 GNU917501:GNU917510 GXQ917501:GXQ917510 HHM917501:HHM917510 HRI917501:HRI917510 IBE917501:IBE917510 ILA917501:ILA917510 IUW917501:IUW917510 JES917501:JES917510 JOO917501:JOO917510 JYK917501:JYK917510 KIG917501:KIG917510 KSC917501:KSC917510 LBY917501:LBY917510 LLU917501:LLU917510 LVQ917501:LVQ917510 MFM917501:MFM917510 MPI917501:MPI917510 MZE917501:MZE917510 NJA917501:NJA917510 NSW917501:NSW917510 OCS917501:OCS917510 OMO917501:OMO917510 OWK917501:OWK917510 PGG917501:PGG917510 PQC917501:PQC917510 PZY917501:PZY917510 QJU917501:QJU917510 QTQ917501:QTQ917510 RDM917501:RDM917510 RNI917501:RNI917510 RXE917501:RXE917510 SHA917501:SHA917510 SQW917501:SQW917510 TAS917501:TAS917510 TKO917501:TKO917510 TUK917501:TUK917510 UEG917501:UEG917510 UOC917501:UOC917510 UXY917501:UXY917510 VHU917501:VHU917510 VRQ917501:VRQ917510 WBM917501:WBM917510 WLI917501:WLI917510 WVE917501:WVE917510 IS983037:IS983046 SO983037:SO983046 ACK983037:ACK983046 AMG983037:AMG983046 AWC983037:AWC983046 BFY983037:BFY983046 BPU983037:BPU983046 BZQ983037:BZQ983046 CJM983037:CJM983046 CTI983037:CTI983046 DDE983037:DDE983046 DNA983037:DNA983046 DWW983037:DWW983046 EGS983037:EGS983046 EQO983037:EQO983046 FAK983037:FAK983046 FKG983037:FKG983046 FUC983037:FUC983046 GDY983037:GDY983046 GNU983037:GNU983046 GXQ983037:GXQ983046 HHM983037:HHM983046 HRI983037:HRI983046 IBE983037:IBE983046 ILA983037:ILA983046 IUW983037:IUW983046 JES983037:JES983046 JOO983037:JOO983046 JYK983037:JYK983046 KIG983037:KIG983046 KSC983037:KSC983046 LBY983037:LBY983046 LLU983037:LLU983046 LVQ983037:LVQ983046 MFM983037:MFM983046 MPI983037:MPI983046 MZE983037:MZE983046 NJA983037:NJA983046 NSW983037:NSW983046 OCS983037:OCS983046 OMO983037:OMO983046 OWK983037:OWK983046 PGG983037:PGG983046 PQC983037:PQC983046 PZY983037:PZY983046 QJU983037:QJU983046 QTQ983037:QTQ983046 RDM983037:RDM983046 RNI983037:RNI983046 RXE983037:RXE983046 SHA983037:SHA983046 SQW983037:SQW983046 TAS983037:TAS983046 TKO983037:TKO983046 TUK983037:TUK983046 UEG983037:UEG983046 UOC983037:UOC983046 UXY983037:UXY983046 VHU983037:VHU983046 VRQ983037:VRQ983046 WBM983037:WBM983046 WLI983037:WLI983046 WVE983037:WVE983046 SO5:SO8 ACK5:ACK8 AMG5:AMG8 AWC5:AWC8 BFY5:BFY8 BPU5:BPU8 BZQ5:BZQ8 CJM5:CJM8 CTI5:CTI8 DDE5:DDE8 DNA5:DNA8 DWW5:DWW8 EGS5:EGS8 EQO5:EQO8 FAK5:FAK8 FKG5:FKG8 FUC5:FUC8 GDY5:GDY8 GNU5:GNU8 GXQ5:GXQ8 HHM5:HHM8 HRI5:HRI8 IBE5:IBE8 ILA5:ILA8 IUW5:IUW8 JES5:JES8 JOO5:JOO8 JYK5:JYK8 KIG5:KIG8 KSC5:KSC8 LBY5:LBY8 LLU5:LLU8 LVQ5:LVQ8 MFM5:MFM8 MPI5:MPI8 MZE5:MZE8 NJA5:NJA8 NSW5:NSW8 OCS5:OCS8 OMO5:OMO8 OWK5:OWK8 PGG5:PGG8 PQC5:PQC8 PZY5:PZY8 QJU5:QJU8 QTQ5:QTQ8 RDM5:RDM8 RNI5:RNI8 RXE5:RXE8 SHA5:SHA8 SQW5:SQW8 TAS5:TAS8 TKO5:TKO8 TUK5:TUK8 UEG5:UEG8 UOC5:UOC8 UXY5:UXY8 VHU5:VHU8 VRQ5:VRQ8 WBM5:WBM8 WLI5:WLI8 WVE5:WVE8 IS5:IS8 SO15:SO18 ACK15:ACK18 AMG15:AMG18 AWC15:AWC18 BFY15:BFY18 BPU15:BPU18 BZQ15:BZQ18 CJM15:CJM18 CTI15:CTI18 DDE15:DDE18 DNA15:DNA18 DWW15:DWW18 EGS15:EGS18 EQO15:EQO18 FAK15:FAK18 FKG15:FKG18 FUC15:FUC18 GDY15:GDY18 GNU15:GNU18 GXQ15:GXQ18 HHM15:HHM18 HRI15:HRI18 IBE15:IBE18 ILA15:ILA18 IUW15:IUW18 JES15:JES18 JOO15:JOO18 JYK15:JYK18 KIG15:KIG18 KSC15:KSC18 LBY15:LBY18 LLU15:LLU18 LVQ15:LVQ18 MFM15:MFM18 MPI15:MPI18 MZE15:MZE18 NJA15:NJA18 NSW15:NSW18 OCS15:OCS18 OMO15:OMO18 OWK15:OWK18 PGG15:PGG18 PQC15:PQC18 PZY15:PZY18 QJU15:QJU18 QTQ15:QTQ18 RDM15:RDM18 RNI15:RNI18 RXE15:RXE18 SHA15:SHA18 SQW15:SQW18 TAS15:TAS18 TKO15:TKO18 TUK15:TUK18 UEG15:UEG18 UOC15:UOC18 UXY15:UXY18 VHU15:VHU18 VRQ15:VRQ18 WBM15:WBM18 WLI15:WLI18 WVE15:WVE18 IS15:IS18">

</xml_diff>